<commit_message>
att attribute input at class node.
</commit_message>
<xml_diff>
--- a/helper ANN/MLP/simplified.weather.numeric.xlsx
+++ b/helper ANN/MLP/simplified.weather.numeric.xlsx
@@ -319,26 +319,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +357,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,7 +719,7 @@
   <dimension ref="K1:CP13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CU9" sqref="CU9"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,236 +733,236 @@
   <sheetData>
     <row r="1" spans="11:94" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="15">
+      <c r="L2" s="13">
         <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="15">
-        <v>0.1</v>
+      <c r="L3" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K4" s="23" t="s">
+      <c r="K4" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K6" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" s="13" t="s">
+      <c r="K6" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="13" t="s">
+      <c r="N6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O6" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="24" t="s">
+      <c r="P6" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="25"/>
-      <c r="AE6" s="25"/>
-      <c r="AF6" s="25"/>
-      <c r="AG6" s="25"/>
-      <c r="AH6" s="25"/>
-      <c r="AI6" s="25"/>
-      <c r="AJ6" s="25"/>
-      <c r="AK6" s="25"/>
-      <c r="AL6" s="25"/>
-      <c r="AM6" s="25"/>
-      <c r="AN6" s="25"/>
-      <c r="AO6" s="25"/>
-      <c r="AP6" s="25"/>
-      <c r="AQ6" s="26"/>
-      <c r="AR6" s="16" t="s">
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="23"/>
+      <c r="AB6" s="23"/>
+      <c r="AC6" s="23"/>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="23"/>
+      <c r="AG6" s="23"/>
+      <c r="AH6" s="23"/>
+      <c r="AI6" s="23"/>
+      <c r="AJ6" s="23"/>
+      <c r="AK6" s="23"/>
+      <c r="AL6" s="23"/>
+      <c r="AM6" s="23"/>
+      <c r="AN6" s="23"/>
+      <c r="AO6" s="23"/>
+      <c r="AP6" s="23"/>
+      <c r="AQ6" s="24"/>
+      <c r="AR6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="AS6" s="16"/>
-      <c r="AT6" s="16"/>
-      <c r="AU6" s="16"/>
-      <c r="AV6" s="16"/>
-      <c r="AW6" s="16"/>
-      <c r="AX6" s="16"/>
-      <c r="AY6" s="16"/>
-      <c r="AZ6" s="16"/>
-      <c r="BA6" s="16"/>
-      <c r="BB6" s="16"/>
-      <c r="BC6" s="16"/>
-      <c r="BD6" s="16"/>
-      <c r="BE6" s="16"/>
-      <c r="BF6" s="16"/>
-      <c r="BG6" s="16"/>
-      <c r="BH6" s="16"/>
-      <c r="BI6" s="16"/>
-      <c r="BJ6" s="16"/>
-      <c r="BK6" s="16"/>
-      <c r="BL6" s="16"/>
-      <c r="BM6" s="16"/>
-      <c r="BN6" s="16"/>
-      <c r="BO6" s="16"/>
-      <c r="BP6" s="16"/>
-      <c r="BQ6" s="16"/>
-      <c r="BR6" s="16"/>
-      <c r="BS6" s="16"/>
-      <c r="BT6" s="16"/>
-      <c r="BU6" s="16"/>
-      <c r="BV6" s="16"/>
-      <c r="BW6" s="16"/>
-      <c r="BX6" s="16"/>
-      <c r="BY6" s="16"/>
-      <c r="BZ6" s="16"/>
-      <c r="CA6" s="16"/>
-      <c r="CB6" s="16"/>
-      <c r="CC6" s="16"/>
-      <c r="CD6" s="16"/>
-      <c r="CE6" s="16"/>
-      <c r="CF6" s="16"/>
-      <c r="CG6" s="16"/>
-      <c r="CH6" s="16"/>
-      <c r="CI6" s="16"/>
-      <c r="CJ6" s="16"/>
-      <c r="CK6" s="16"/>
-      <c r="CL6" s="16"/>
-      <c r="CM6" s="16"/>
-      <c r="CN6" s="16"/>
-      <c r="CO6" s="16"/>
-      <c r="CP6" s="16"/>
+      <c r="AS6" s="21"/>
+      <c r="AT6" s="21"/>
+      <c r="AU6" s="21"/>
+      <c r="AV6" s="21"/>
+      <c r="AW6" s="21"/>
+      <c r="AX6" s="21"/>
+      <c r="AY6" s="21"/>
+      <c r="AZ6" s="21"/>
+      <c r="BA6" s="21"/>
+      <c r="BB6" s="21"/>
+      <c r="BC6" s="21"/>
+      <c r="BD6" s="21"/>
+      <c r="BE6" s="21"/>
+      <c r="BF6" s="21"/>
+      <c r="BG6" s="21"/>
+      <c r="BH6" s="21"/>
+      <c r="BI6" s="21"/>
+      <c r="BJ6" s="21"/>
+      <c r="BK6" s="21"/>
+      <c r="BL6" s="21"/>
+      <c r="BM6" s="21"/>
+      <c r="BN6" s="21"/>
+      <c r="BO6" s="21"/>
+      <c r="BP6" s="21"/>
+      <c r="BQ6" s="21"/>
+      <c r="BR6" s="21"/>
+      <c r="BS6" s="21"/>
+      <c r="BT6" s="21"/>
+      <c r="BU6" s="21"/>
+      <c r="BV6" s="21"/>
+      <c r="BW6" s="21"/>
+      <c r="BX6" s="21"/>
+      <c r="BY6" s="21"/>
+      <c r="BZ6" s="21"/>
+      <c r="CA6" s="21"/>
+      <c r="CB6" s="21"/>
+      <c r="CC6" s="21"/>
+      <c r="CD6" s="21"/>
+      <c r="CE6" s="21"/>
+      <c r="CF6" s="21"/>
+      <c r="CG6" s="21"/>
+      <c r="CH6" s="21"/>
+      <c r="CI6" s="21"/>
+      <c r="CJ6" s="21"/>
+      <c r="CK6" s="21"/>
+      <c r="CL6" s="21"/>
+      <c r="CM6" s="21"/>
+      <c r="CN6" s="21"/>
+      <c r="CO6" s="21"/>
+      <c r="CP6" s="21"/>
     </row>
     <row r="7" spans="11:94" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="17" t="s">
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17" t="s">
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
-      <c r="AA7" s="17"/>
-      <c r="AB7" s="17"/>
-      <c r="AC7" s="17"/>
-      <c r="AD7" s="17" t="s">
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="AE7" s="17"/>
-      <c r="AF7" s="17"/>
-      <c r="AG7" s="17"/>
-      <c r="AH7" s="17"/>
-      <c r="AI7" s="17"/>
-      <c r="AJ7" s="17"/>
-      <c r="AK7" s="27" t="s">
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" s="20"/>
+      <c r="AK7" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="AL7" s="28"/>
-      <c r="AM7" s="28"/>
-      <c r="AN7" s="28"/>
-      <c r="AO7" s="28"/>
-      <c r="AP7" s="28"/>
-      <c r="AQ7" s="29"/>
-      <c r="AR7" s="17" t="s">
+      <c r="AL7" s="26"/>
+      <c r="AM7" s="26"/>
+      <c r="AN7" s="26"/>
+      <c r="AO7" s="26"/>
+      <c r="AP7" s="26"/>
+      <c r="AQ7" s="27"/>
+      <c r="AR7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AS7" s="17"/>
-      <c r="AT7" s="17"/>
-      <c r="AU7" s="17"/>
-      <c r="AV7" s="17"/>
-      <c r="AW7" s="17"/>
-      <c r="AX7" s="17"/>
-      <c r="AY7" s="17"/>
-      <c r="AZ7" s="17"/>
-      <c r="BA7" s="17"/>
-      <c r="BB7" s="17"/>
-      <c r="BC7" s="17"/>
-      <c r="BD7" s="17"/>
-      <c r="BE7" s="17"/>
-      <c r="BF7" s="17"/>
-      <c r="BG7" s="17"/>
-      <c r="BH7" s="17"/>
-      <c r="BI7" s="17" t="s">
+      <c r="AS7" s="20"/>
+      <c r="AT7" s="20"/>
+      <c r="AU7" s="20"/>
+      <c r="AV7" s="20"/>
+      <c r="AW7" s="20"/>
+      <c r="AX7" s="20"/>
+      <c r="AY7" s="20"/>
+      <c r="AZ7" s="20"/>
+      <c r="BA7" s="20"/>
+      <c r="BB7" s="20"/>
+      <c r="BC7" s="20"/>
+      <c r="BD7" s="20"/>
+      <c r="BE7" s="20"/>
+      <c r="BF7" s="20"/>
+      <c r="BG7" s="20"/>
+      <c r="BH7" s="20"/>
+      <c r="BI7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="BJ7" s="17"/>
-      <c r="BK7" s="17"/>
-      <c r="BL7" s="17"/>
-      <c r="BM7" s="17"/>
-      <c r="BN7" s="17"/>
-      <c r="BO7" s="17"/>
-      <c r="BP7" s="17"/>
-      <c r="BQ7" s="17"/>
-      <c r="BR7" s="17"/>
-      <c r="BS7" s="17"/>
-      <c r="BT7" s="17"/>
-      <c r="BU7" s="17"/>
-      <c r="BV7" s="17"/>
-      <c r="BW7" s="17"/>
-      <c r="BX7" s="17"/>
-      <c r="BY7" s="17"/>
-      <c r="BZ7" s="17" t="s">
+      <c r="BJ7" s="20"/>
+      <c r="BK7" s="20"/>
+      <c r="BL7" s="20"/>
+      <c r="BM7" s="20"/>
+      <c r="BN7" s="20"/>
+      <c r="BO7" s="20"/>
+      <c r="BP7" s="20"/>
+      <c r="BQ7" s="20"/>
+      <c r="BR7" s="20"/>
+      <c r="BS7" s="20"/>
+      <c r="BT7" s="20"/>
+      <c r="BU7" s="20"/>
+      <c r="BV7" s="20"/>
+      <c r="BW7" s="20"/>
+      <c r="BX7" s="20"/>
+      <c r="BY7" s="20"/>
+      <c r="BZ7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="CA7" s="17"/>
-      <c r="CB7" s="17"/>
-      <c r="CC7" s="17"/>
-      <c r="CD7" s="17"/>
-      <c r="CE7" s="17"/>
-      <c r="CF7" s="17"/>
-      <c r="CG7" s="17"/>
-      <c r="CH7" s="17"/>
-      <c r="CI7" s="17"/>
-      <c r="CJ7" s="17"/>
-      <c r="CK7" s="17"/>
-      <c r="CL7" s="17"/>
-      <c r="CM7" s="17"/>
-      <c r="CN7" s="17"/>
-      <c r="CO7" s="17"/>
-      <c r="CP7" s="17"/>
+      <c r="CA7" s="20"/>
+      <c r="CB7" s="20"/>
+      <c r="CC7" s="20"/>
+      <c r="CD7" s="20"/>
+      <c r="CE7" s="20"/>
+      <c r="CF7" s="20"/>
+      <c r="CG7" s="20"/>
+      <c r="CH7" s="20"/>
+      <c r="CI7" s="20"/>
+      <c r="CJ7" s="20"/>
+      <c r="CK7" s="20"/>
+      <c r="CL7" s="20"/>
+      <c r="CM7" s="20"/>
+      <c r="CN7" s="20"/>
+      <c r="CO7" s="20"/>
+      <c r="CP7" s="20"/>
     </row>
     <row r="8" spans="11:94" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
       <c r="P8" s="2">
         <v>0</v>
       </c>
@@ -1047,162 +1047,162 @@
       <c r="AQ8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AR8" s="21" t="s">
+      <c r="AR8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="AS8" s="21" t="s">
+      <c r="AS8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="AT8" s="22" t="s">
+      <c r="AT8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="AU8" s="22" t="s">
+      <c r="AU8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="AV8" s="22" t="s">
+      <c r="AV8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="AW8" s="22" t="s">
+      <c r="AW8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="AX8" s="22" t="s">
+      <c r="AX8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="AY8" s="22" t="s">
+      <c r="AY8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AZ8" s="22" t="s">
+      <c r="AZ8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="BA8" s="22" t="s">
+      <c r="BA8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="BB8" s="22" t="s">
+      <c r="BB8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="BC8" s="22" t="s">
+      <c r="BC8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="BD8" s="22" t="s">
+      <c r="BD8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="BE8" s="22" t="s">
+      <c r="BE8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="BF8" s="22" t="s">
+      <c r="BF8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="BG8" s="22" t="s">
+      <c r="BG8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="BH8" s="22" t="s">
+      <c r="BH8" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="BI8" s="21" t="s">
+      <c r="BI8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="BJ8" s="21" t="s">
+      <c r="BJ8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="BK8" s="22" t="s">
+      <c r="BK8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="BL8" s="22" t="s">
+      <c r="BL8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="BM8" s="22" t="s">
+      <c r="BM8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="BN8" s="22" t="s">
+      <c r="BN8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="BO8" s="22" t="s">
+      <c r="BO8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="BP8" s="22" t="s">
+      <c r="BP8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="BQ8" s="22" t="s">
+      <c r="BQ8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="BR8" s="22" t="s">
+      <c r="BR8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="BS8" s="22" t="s">
+      <c r="BS8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="BT8" s="22" t="s">
+      <c r="BT8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="BU8" s="22" t="s">
+      <c r="BU8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="BV8" s="22" t="s">
+      <c r="BV8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="BW8" s="22" t="s">
+      <c r="BW8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="BX8" s="22" t="s">
+      <c r="BX8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="BY8" s="22" t="s">
+      <c r="BY8" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="BZ8" s="21" t="s">
+      <c r="BZ8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="CA8" s="21" t="s">
+      <c r="CA8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="CB8" s="22" t="s">
+      <c r="CB8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="CC8" s="22" t="s">
+      <c r="CC8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="CD8" s="22" t="s">
+      <c r="CD8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="CE8" s="22" t="s">
+      <c r="CE8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="CF8" s="22" t="s">
+      <c r="CF8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="CG8" s="22" t="s">
+      <c r="CG8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="CH8" s="22" t="s">
+      <c r="CH8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="CI8" s="22" t="s">
+      <c r="CI8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="CJ8" s="22" t="s">
+      <c r="CJ8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="CK8" s="22" t="s">
+      <c r="CK8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="CL8" s="22" t="s">
+      <c r="CL8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="CM8" s="22" t="s">
+      <c r="CM8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="CN8" s="22" t="s">
+      <c r="CN8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="CO8" s="22" t="s">
+      <c r="CO8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="CP8" s="22" t="s">
+      <c r="CP8" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K9" s="14">
+      <c r="K9" s="29">
         <v>1</v>
       </c>
       <c r="L9" s="10">
@@ -1217,9 +1217,9 @@
       <c r="O9" s="10">
         <v>1</v>
       </c>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
       <c r="S9" s="4">
         <f>AR9*W9+AT9*X9+AV9*Y9+$L$4*BE9</f>
         <v>0</v>
@@ -1264,11 +1264,11 @@
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="AD9" s="18"/>
-      <c r="AE9" s="18"/>
-      <c r="AF9" s="18"/>
-      <c r="AG9" s="18"/>
-      <c r="AH9" s="18"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+      <c r="AH9" s="14"/>
       <c r="AI9" s="4">
         <v>0</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="BX9" s="4">
-        <f t="shared" ref="BX9:BY12" si="2">$L$2*AP9*$L$4</f>
+        <f t="shared" ref="BX9:BY9" si="2">$L$2*AP9*$L$4</f>
         <v>-1.2500000000000001E-2</v>
       </c>
       <c r="BY9" s="4">
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="10" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K10" s="14"/>
+      <c r="K10" s="29"/>
       <c r="L10" s="11">
         <v>80</v>
       </c>
@@ -1496,9 +1496,9 @@
       <c r="O10" s="11">
         <v>1</v>
       </c>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
       <c r="S10" s="8">
         <f t="shared" ref="S10:S12" si="4">AR10*W10+AT10*X10+AV10*Y10+$L$4*BE10</f>
         <v>0</v>
@@ -1543,11 +1543,11 @@
         <f t="shared" ref="AC10:AC12" si="14">1/(1+EXP(-V10))</f>
         <v>0.50468736267572623</v>
       </c>
-      <c r="AD10" s="19"/>
-      <c r="AE10" s="19"/>
-      <c r="AF10" s="19"/>
-      <c r="AG10" s="19"/>
-      <c r="AH10" s="19"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="15"/>
+      <c r="AF10" s="15"/>
+      <c r="AG10" s="15"/>
+      <c r="AH10" s="15"/>
       <c r="AI10" s="8">
         <v>0</v>
       </c>
@@ -1676,30 +1676,30 @@
       </c>
       <c r="BO10" s="8">
         <f>$L$2*AP10*Z10+BO9*$L$3</f>
-        <v>-6.8158638317207913E-3</v>
+        <v>-6.1908638317207908E-3</v>
       </c>
       <c r="BP10" s="8">
         <f>$L$2*AQ10*Z10+BP9*$L$3</f>
-        <v>6.8158638317207931E-3</v>
+        <v>6.1908638317207925E-3</v>
       </c>
       <c r="BQ10" s="8">
         <f>$L$2*AP10*AA10+BQ9*$L$3</f>
-        <v>-6.8158638317207913E-3</v>
+        <v>-6.1908638317207908E-3</v>
       </c>
       <c r="BR10" s="8">
         <f>$L$2*AQ10*AA10+BR9*$L$3</f>
-        <v>6.8158638317207931E-3</v>
+        <v>6.1908638317207925E-3</v>
       </c>
       <c r="BS10" s="5">
-        <f t="shared" ref="BS10:BS12" si="38">$L$2*AX10*AG10</f>
+        <f t="shared" ref="BS10" si="38">$L$2*AX10*AG10</f>
         <v>0</v>
       </c>
       <c r="BT10" s="5">
-        <f t="shared" ref="BT10:BT12" si="39">$L$2*AY10*AH10</f>
+        <f t="shared" ref="BT10" si="39">$L$2*AY10*AH10</f>
         <v>0</v>
       </c>
       <c r="BU10" s="5">
-        <f t="shared" ref="BU10:BU12" si="40">$L$2*AZ10*AI10</f>
+        <f t="shared" ref="BU10" si="40">$L$2*AZ10*AI10</f>
         <v>0</v>
       </c>
       <c r="BV10" s="8">
@@ -1712,11 +1712,11 @@
       </c>
       <c r="BX10" s="8">
         <f>$L$2*AP10*$L$4+BX9*$L$3</f>
-        <v>-1.3631727663441583E-2</v>
+        <v>-1.2381727663441582E-2</v>
       </c>
       <c r="BY10" s="8">
         <f>$L$2*AQ10*$L$4+BY9*$L$3</f>
-        <v>1.3631727663441586E-2</v>
+        <v>1.2381727663441585E-2</v>
       </c>
       <c r="BZ10" s="8">
         <f t="shared" ref="BZ10:BZ12" si="41">AR10+BI10</f>
@@ -1744,19 +1744,19 @@
       </c>
       <c r="CF10" s="8">
         <f t="shared" si="3"/>
-        <v>-1.3065863831720792E-2</v>
+        <v>-1.2440863831720791E-2</v>
       </c>
       <c r="CG10" s="8">
         <f t="shared" si="3"/>
-        <v>1.3065863831720793E-2</v>
+        <v>1.2440863831720793E-2</v>
       </c>
       <c r="CH10" s="8">
         <f t="shared" si="3"/>
-        <v>-1.3065863831720792E-2</v>
+        <v>-1.2440863831720791E-2</v>
       </c>
       <c r="CI10" s="8">
         <f t="shared" si="3"/>
-        <v>1.3065863831720793E-2</v>
+        <v>1.2440863831720793E-2</v>
       </c>
       <c r="CJ10" s="5">
         <f t="shared" si="3"/>
@@ -1780,15 +1780,15 @@
       </c>
       <c r="CO10" s="8">
         <f t="shared" si="3"/>
-        <v>-2.6131727663441583E-2</v>
+        <v>-2.4881727663441582E-2</v>
       </c>
       <c r="CP10" s="8">
         <f t="shared" si="3"/>
-        <v>2.6131727663441587E-2</v>
+        <v>2.4881727663441586E-2</v>
       </c>
     </row>
     <row r="11" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K11" s="14"/>
+      <c r="K11" s="29"/>
       <c r="L11" s="11">
         <v>83</v>
       </c>
@@ -1801,9 +1801,9 @@
       <c r="O11" s="11">
         <v>0</v>
       </c>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
       <c r="S11" s="8">
         <f t="shared" si="4"/>
         <v>0.55644257977485445</v>
@@ -1814,11 +1814,11 @@
       </c>
       <c r="U11" s="8">
         <f t="shared" si="6"/>
-        <v>-4.2741812187511496E-2</v>
+        <v>-4.0697275908758886E-2</v>
       </c>
       <c r="V11" s="8">
         <f t="shared" si="7"/>
-        <v>4.2741812187511496E-2</v>
+        <v>4.0697275908758893E-2</v>
       </c>
       <c r="W11" s="11">
         <f t="shared" si="8"/>
@@ -1842,17 +1842,17 @@
       </c>
       <c r="AB11" s="8">
         <f t="shared" si="13"/>
-        <v>0.48931617339379146</v>
+        <v>0.4898270850737334</v>
       </c>
       <c r="AC11" s="8">
         <f t="shared" si="14"/>
-        <v>0.51068382660620859</v>
-      </c>
-      <c r="AD11" s="19"/>
-      <c r="AE11" s="19"/>
-      <c r="AF11" s="19"/>
-      <c r="AG11" s="19"/>
-      <c r="AH11" s="19"/>
+        <v>0.5101729149262666</v>
+      </c>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="15"/>
+      <c r="AF11" s="15"/>
+      <c r="AG11" s="15"/>
+      <c r="AH11" s="15"/>
       <c r="AI11" s="8">
         <v>1</v>
       </c>
@@ -1861,11 +1861,11 @@
       </c>
       <c r="AK11" s="8">
         <f t="shared" si="15"/>
-        <v>3.2542625977694577E-2</v>
+        <v>3.0956283635477134E-2</v>
       </c>
       <c r="AL11" s="8">
         <f t="shared" si="16"/>
-        <v>3.9321542812821887E-2</v>
+        <v>3.7404751329305777E-2</v>
       </c>
       <c r="AM11" s="8">
         <f t="shared" si="17"/>
@@ -1873,19 +1873,19 @@
       </c>
       <c r="AN11" s="8">
         <f t="shared" si="18"/>
-        <v>-7.723415478546017E-4</v>
+        <v>-7.346925240525493E-4</v>
       </c>
       <c r="AO11" s="8">
         <f t="shared" si="19"/>
-        <v>-7.723415478546017E-4</v>
+        <v>-7.346925240525493E-4</v>
       </c>
       <c r="AP11" s="8">
         <f t="shared" si="20"/>
-        <v>0.12761266507975952</v>
+        <v>0.12749043185588302</v>
       </c>
       <c r="AQ11" s="8">
         <f t="shared" si="21"/>
-        <v>-0.12761266507975949</v>
+        <v>-0.12749043185588302</v>
       </c>
       <c r="AR11" s="8">
         <f t="shared" ref="AR11:AR12" si="42">BZ10</f>
@@ -1913,19 +1913,19 @@
       </c>
       <c r="AX11" s="8">
         <f t="shared" si="27"/>
-        <v>-1.3065863831720792E-2</v>
+        <v>-1.2440863831720791E-2</v>
       </c>
       <c r="AY11" s="8">
         <f t="shared" si="28"/>
-        <v>1.3065863831720793E-2</v>
+        <v>1.2440863831720793E-2</v>
       </c>
       <c r="AZ11" s="8">
         <f t="shared" si="29"/>
-        <v>-1.3065863831720792E-2</v>
+        <v>-1.2440863831720791E-2</v>
       </c>
       <c r="BA11" s="8">
         <f t="shared" si="30"/>
-        <v>1.3065863831720793E-2</v>
+        <v>1.2440863831720793E-2</v>
       </c>
       <c r="BB11" s="5">
         <f t="shared" si="31"/>
@@ -1949,51 +1949,51 @@
       </c>
       <c r="BG11" s="8">
         <f t="shared" si="36"/>
-        <v>-2.6131727663441583E-2</v>
+        <v>-2.4881727663441582E-2</v>
       </c>
       <c r="BH11" s="8">
         <f t="shared" si="37"/>
-        <v>2.6131727663441587E-2</v>
+        <v>2.4881727663441586E-2</v>
       </c>
       <c r="BI11" s="8">
         <f t="shared" ref="BI11:BI12" si="43">$L$2*AN11*W11+$L$3*BI10</f>
-        <v>-6.1008916556071551E-3</v>
+        <v>-6.0979479496361599E-3</v>
       </c>
       <c r="BJ11" s="8">
         <f t="shared" ref="BJ11:BJ12" si="44">$L$2*AO11*W11+$L$3*BJ10</f>
-        <v>-6.1008916556071551E-3</v>
+        <v>-6.0979479496361599E-3</v>
       </c>
       <c r="BK11" s="8">
         <f t="shared" ref="BK11:BK12" si="45">$L$2*AN11*X11+BK10*$L$3</f>
-        <v>-6.2939012210152809E-3</v>
+        <v>-6.3183557068519245E-3</v>
       </c>
       <c r="BL11" s="8">
         <f t="shared" ref="BL11:BL12" si="46">$L$2*AO11*X11+BL10*$L$3</f>
-        <v>-6.2939012210152809E-3</v>
+        <v>-6.3183557068519245E-3</v>
       </c>
       <c r="BM11" s="8">
         <f t="shared" ref="BM11:BM12" si="47">$L$2*AN11*Y11+BM10*$L$3</f>
-        <v>-7.7234154785460178E-5</v>
+        <v>-7.3469252405254938E-5</v>
       </c>
       <c r="BN11" s="8">
         <f t="shared" ref="BN11:BN12" si="48">$L$2*AO11*Y11+BN10*$L$3</f>
-        <v>-7.7234154785460178E-5</v>
+        <v>-7.3469252405254938E-5</v>
       </c>
       <c r="BO11" s="8">
         <f t="shared" ref="BO11:BO12" si="49">$L$2*AP11*Z11+BO10*$L$3</f>
-        <v>7.4298449795618948E-3</v>
+        <v>8.1036618642668715E-3</v>
       </c>
       <c r="BP11" s="8">
         <f t="shared" ref="BP11:BP12" si="50">$L$2*AQ11*Z11+BP10*$L$3</f>
-        <v>-7.4298449795618905E-3</v>
+        <v>-8.1036618642668715E-3</v>
       </c>
       <c r="BQ11" s="8">
         <f t="shared" ref="BQ11:BQ12" si="51">$L$2*AP11*AA11+BQ10*$L$3</f>
-        <v>7.4298449795618948E-3</v>
+        <v>8.1036618642668715E-3</v>
       </c>
       <c r="BR11" s="8">
         <f t="shared" ref="BR11:BR12" si="52">$L$2*AQ11*AA11+BR10*$L$3</f>
-        <v>-7.4298449795618905E-3</v>
+        <v>-8.1036618642668715E-3</v>
       </c>
       <c r="BS11" s="5">
         <f t="shared" ref="BS11:BS12" si="53">$L$2*AX11*AG11</f>
@@ -2005,63 +2005,63 @@
       </c>
       <c r="BU11" s="5">
         <f t="shared" ref="BU11:BU12" si="55">$L$2*AZ11*AI11</f>
-        <v>-1.3065863831720793E-3</v>
+        <v>-1.2440863831720793E-3</v>
       </c>
       <c r="BV11" s="8">
         <f t="shared" ref="BV11:BV12" si="56">$L$2*AN11*$L$4+BV10*$L$3</f>
-        <v>-7.3364864890634681E-5</v>
+        <v>-7.3469252405254938E-5</v>
       </c>
       <c r="BW11" s="8">
         <f t="shared" ref="BW11:BW12" si="57">$L$2*AO11*$L$4+BW10*$L$3</f>
-        <v>-7.3364864890634681E-5</v>
+        <v>-7.3469252405254938E-5</v>
       </c>
       <c r="BX11" s="8">
         <f t="shared" ref="BX11:BX12" si="58">$L$2*AP11*$L$4+BX10*$L$3</f>
-        <v>1.1398093741631796E-2</v>
+        <v>1.2749043185588303E-2</v>
       </c>
       <c r="BY11" s="8">
         <f t="shared" ref="BY11:BY12" si="59">$L$2*AQ11*$L$4+BY10*$L$3</f>
-        <v>-1.139809374163179E-2</v>
+        <v>-1.2749043185588303E-2</v>
       </c>
       <c r="BZ11" s="8">
         <f t="shared" si="41"/>
-        <v>-3.0054597397467593E-3</v>
+        <v>-3.0025160337757641E-3</v>
       </c>
       <c r="CA11" s="8">
         <f t="shared" si="3"/>
-        <v>-3.0054597397467593E-3</v>
+        <v>-3.0025160337757641E-3</v>
       </c>
       <c r="CB11" s="8">
         <f t="shared" si="3"/>
-        <v>-2.8115403156723355E-3</v>
+        <v>-2.8359948015089791E-3</v>
       </c>
       <c r="CC11" s="8">
         <f t="shared" si="3"/>
-        <v>-2.8115403156723355E-3</v>
+        <v>-2.8359948015089791E-3</v>
       </c>
       <c r="CD11" s="8">
         <f t="shared" si="3"/>
-        <v>-7.7234154785460178E-5</v>
+        <v>-7.3469252405254938E-5</v>
       </c>
       <c r="CE11" s="8">
         <f t="shared" si="3"/>
-        <v>-7.7234154785460178E-5</v>
+        <v>-7.3469252405254938E-5</v>
       </c>
       <c r="CF11" s="8">
         <f t="shared" si="3"/>
-        <v>-5.6360188521588968E-3</v>
+        <v>-4.3372019674539197E-3</v>
       </c>
       <c r="CG11" s="8">
         <f t="shared" si="3"/>
-        <v>5.6360188521589029E-3</v>
+        <v>4.3372019674539214E-3</v>
       </c>
       <c r="CH11" s="8">
         <f t="shared" si="3"/>
-        <v>-5.6360188521588968E-3</v>
+        <v>-4.3372019674539197E-3</v>
       </c>
       <c r="CI11" s="8">
         <f t="shared" si="3"/>
-        <v>5.6360188521589029E-3</v>
+        <v>4.3372019674539214E-3</v>
       </c>
       <c r="CJ11" s="5">
         <f t="shared" si="3"/>
@@ -2073,27 +2073,27 @@
       </c>
       <c r="CL11" s="5">
         <f t="shared" si="3"/>
-        <v>-1.3065863831720793E-3</v>
+        <v>-1.2440863831720793E-3</v>
       </c>
       <c r="CM11" s="8">
         <f t="shared" si="3"/>
-        <v>-3.4671965942379733E-5</v>
+        <v>-3.477635345699999E-5</v>
       </c>
       <c r="CN11" s="8">
         <f t="shared" si="3"/>
-        <v>-3.4671965942379733E-5</v>
+        <v>-3.477635345699999E-5</v>
       </c>
       <c r="CO11" s="8">
         <f t="shared" si="3"/>
-        <v>-1.4733633921809788E-2</v>
+        <v>-1.2132684477853279E-2</v>
       </c>
       <c r="CP11" s="8">
         <f t="shared" si="3"/>
-        <v>1.4733633921809796E-2</v>
+        <v>1.2132684477853282E-2</v>
       </c>
     </row>
     <row r="12" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K12" s="14"/>
+      <c r="K12" s="29"/>
       <c r="L12" s="6">
         <v>70</v>
       </c>
@@ -2106,24 +2106,24 @@
       <c r="O12" s="6">
         <v>0</v>
       </c>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
       <c r="S12" s="9">
         <f t="shared" si="4"/>
-        <v>-0.48040195820754522</v>
+        <v>-0.48253986891502776</v>
       </c>
       <c r="T12" s="9">
         <f t="shared" si="5"/>
-        <v>-0.48040195820754522</v>
+        <v>-0.48253986891502776</v>
       </c>
       <c r="U12" s="9">
         <f t="shared" si="6"/>
-        <v>-1.9041324437377535E-2</v>
+        <v>-1.544329287500092E-2</v>
       </c>
       <c r="V12" s="9">
         <f t="shared" si="7"/>
-        <v>1.9041324437377549E-2</v>
+        <v>1.5443292875000927E-2</v>
       </c>
       <c r="W12" s="12">
         <f t="shared" si="8"/>
@@ -2139,25 +2139,25 @@
       </c>
       <c r="Z12" s="9">
         <f t="shared" si="11"/>
-        <v>0.38215721314680051</v>
+        <v>0.38165255180531493</v>
       </c>
       <c r="AA12" s="9">
         <f t="shared" si="12"/>
-        <v>0.38215721314680051</v>
+        <v>0.38165255180531493</v>
       </c>
       <c r="AB12" s="9">
         <f t="shared" si="13"/>
-        <v>0.49523981271568629</v>
+        <v>0.49613925351176752</v>
       </c>
       <c r="AC12" s="9">
         <f t="shared" si="14"/>
-        <v>0.50476018728431382</v>
-      </c>
-      <c r="AD12" s="20"/>
-      <c r="AE12" s="20"/>
-      <c r="AF12" s="20"/>
-      <c r="AG12" s="20"/>
-      <c r="AH12" s="20"/>
+        <v>0.50386074648823254</v>
+      </c>
+      <c r="AD12" s="16"/>
+      <c r="AE12" s="16"/>
+      <c r="AF12" s="16"/>
+      <c r="AG12" s="16"/>
+      <c r="AH12" s="16"/>
       <c r="AI12" s="9">
         <v>1</v>
       </c>
@@ -2166,11 +2166,11 @@
       </c>
       <c r="AK12" s="9">
         <f t="shared" si="15"/>
-        <v>-9.7498122395020936E-3</v>
+        <v>-7.478723676312444E-3</v>
       </c>
       <c r="AL12" s="9">
         <f t="shared" si="16"/>
-        <v>-1.7221753172806952E-2</v>
+        <v>-1.3338140565415976E-2</v>
       </c>
       <c r="AM12" s="9">
         <f t="shared" si="17"/>
@@ -2178,59 +2178,59 @@
       </c>
       <c r="AN12" s="9">
         <f t="shared" si="18"/>
-        <v>-3.3582127883264668E-4</v>
+        <v>-2.5784874713035121E-4</v>
       </c>
       <c r="AO12" s="9">
         <f t="shared" si="19"/>
-        <v>-3.3582127883264668E-4</v>
+        <v>-2.5784874713035121E-4</v>
       </c>
       <c r="AP12" s="9">
         <f t="shared" si="20"/>
-        <v>0.12617860926668081</v>
+        <v>0.12595767639450536</v>
       </c>
       <c r="AQ12" s="9">
         <f t="shared" si="21"/>
-        <v>-0.12617860926668084</v>
+        <v>-0.12595767639450536</v>
       </c>
       <c r="AR12" s="9">
         <f t="shared" si="42"/>
-        <v>-3.0054597397467593E-3</v>
+        <v>-3.0025160337757641E-3</v>
       </c>
       <c r="AS12" s="9">
         <f t="shared" si="22"/>
-        <v>-3.0054597397467593E-3</v>
+        <v>-3.0025160337757641E-3</v>
       </c>
       <c r="AT12" s="9">
         <f t="shared" si="23"/>
-        <v>-2.8115403156723355E-3</v>
+        <v>-2.8359948015089791E-3</v>
       </c>
       <c r="AU12" s="9">
         <f t="shared" si="24"/>
-        <v>-2.8115403156723355E-3</v>
+        <v>-2.8359948015089791E-3</v>
       </c>
       <c r="AV12" s="9">
         <f t="shared" si="25"/>
-        <v>-7.7234154785460178E-5</v>
+        <v>-7.3469252405254938E-5</v>
       </c>
       <c r="AW12" s="9">
         <f t="shared" si="26"/>
-        <v>-7.7234154785460178E-5</v>
+        <v>-7.3469252405254938E-5</v>
       </c>
       <c r="AX12" s="9">
         <f t="shared" si="27"/>
-        <v>-5.6360188521588968E-3</v>
+        <v>-4.3372019674539197E-3</v>
       </c>
       <c r="AY12" s="9">
         <f t="shared" si="28"/>
-        <v>5.6360188521589029E-3</v>
+        <v>4.3372019674539214E-3</v>
       </c>
       <c r="AZ12" s="9">
         <f t="shared" si="29"/>
-        <v>-5.6360188521588968E-3</v>
+        <v>-4.3372019674539197E-3</v>
       </c>
       <c r="BA12" s="9">
         <f t="shared" si="30"/>
-        <v>5.6360188521589029E-3</v>
+        <v>4.3372019674539214E-3</v>
       </c>
       <c r="BB12" s="7">
         <f t="shared" si="31"/>
@@ -2242,63 +2242,63 @@
       </c>
       <c r="BD12" s="7">
         <f t="shared" si="33"/>
-        <v>-1.3065863831720793E-3</v>
+        <v>-1.2440863831720793E-3</v>
       </c>
       <c r="BE12" s="9">
         <f t="shared" si="34"/>
-        <v>-3.4671965942379733E-5</v>
+        <v>-3.477635345699999E-5</v>
       </c>
       <c r="BF12" s="9">
         <f t="shared" si="35"/>
-        <v>-3.4671965942379733E-5</v>
+        <v>-3.477635345699999E-5</v>
       </c>
       <c r="BG12" s="9">
         <f t="shared" si="36"/>
-        <v>-1.4733633921809788E-2</v>
+        <v>-1.2132684477853279E-2</v>
       </c>
       <c r="BH12" s="9">
         <f t="shared" si="37"/>
-        <v>1.4733633921809796E-2</v>
+        <v>1.2132684477853282E-2</v>
       </c>
       <c r="BI12" s="9">
         <f t="shared" si="43"/>
-        <v>-2.9608381173892428E-3</v>
+        <v>-1.8049412299124587E-3</v>
       </c>
       <c r="BJ12" s="9">
         <f t="shared" si="44"/>
-        <v>-2.9608381173892428E-3</v>
+        <v>-1.8049412299124587E-3</v>
       </c>
       <c r="BK12" s="9">
         <f t="shared" si="45"/>
-        <v>-3.8532743988949365E-3</v>
+        <v>-2.4753479724513717E-3</v>
       </c>
       <c r="BL12" s="9">
         <f t="shared" si="46"/>
-        <v>-3.8532743988949365E-3</v>
+        <v>-2.4753479724513717E-3</v>
       </c>
       <c r="BM12" s="9">
         <f t="shared" si="47"/>
-        <v>-4.130554336181069E-5</v>
+        <v>-2.5784874713035123E-5</v>
       </c>
       <c r="BN12" s="9">
         <f t="shared" si="48"/>
-        <v>-4.130554336181069E-5</v>
+        <v>-2.5784874713035123E-5</v>
       </c>
       <c r="BO12" s="9">
         <f t="shared" si="49"/>
-        <v>5.5649910655655695E-3</v>
+        <v>4.8072068615431056E-3</v>
       </c>
       <c r="BP12" s="9">
         <f t="shared" si="50"/>
-        <v>-5.5649910655655695E-3</v>
+        <v>-4.8072068615431056E-3</v>
       </c>
       <c r="BQ12" s="9">
         <f t="shared" si="51"/>
-        <v>5.5649910655655695E-3</v>
+        <v>4.8072068615431056E-3</v>
       </c>
       <c r="BR12" s="9">
         <f t="shared" si="52"/>
-        <v>-5.5649910655655695E-3</v>
+        <v>-4.8072068615431056E-3</v>
       </c>
       <c r="BS12" s="7">
         <f t="shared" si="53"/>
@@ -2310,63 +2310,63 @@
       </c>
       <c r="BU12" s="7">
         <f t="shared" si="55"/>
-        <v>-5.6360188521588968E-4</v>
+        <v>-4.3372019674539197E-4</v>
       </c>
       <c r="BV12" s="9">
         <f t="shared" si="56"/>
-        <v>-4.0918614372328141E-5</v>
+        <v>-2.5784874713035123E-5</v>
       </c>
       <c r="BW12" s="9">
         <f t="shared" si="57"/>
-        <v>-4.0918614372328141E-5</v>
+        <v>-2.5784874713035123E-5</v>
       </c>
       <c r="BX12" s="9">
         <f t="shared" si="58"/>
-        <v>1.3757670300831262E-2</v>
+        <v>1.2595767639450537E-2</v>
       </c>
       <c r="BY12" s="9">
         <f t="shared" si="59"/>
-        <v>-1.3757670300831262E-2</v>
+        <v>-1.2595767639450537E-2</v>
       </c>
       <c r="BZ12" s="9">
         <f t="shared" si="41"/>
-        <v>-5.9662978571360017E-3</v>
+        <v>-4.8074572636882225E-3</v>
       </c>
       <c r="CA12" s="9">
         <f t="shared" si="3"/>
-        <v>-5.9662978571360017E-3</v>
+        <v>-4.8074572636882225E-3</v>
       </c>
       <c r="CB12" s="9">
         <f t="shared" si="3"/>
-        <v>-6.6648147145672715E-3</v>
+        <v>-5.3113427739603508E-3</v>
       </c>
       <c r="CC12" s="9">
         <f t="shared" si="3"/>
-        <v>-6.6648147145672715E-3</v>
+        <v>-5.3113427739603508E-3</v>
       </c>
       <c r="CD12" s="9">
         <f t="shared" si="3"/>
-        <v>-1.1853969814727087E-4</v>
+        <v>-9.9254127118290065E-5</v>
       </c>
       <c r="CE12" s="9">
         <f t="shared" si="3"/>
-        <v>-1.1853969814727087E-4</v>
+        <v>-9.9254127118290065E-5</v>
       </c>
       <c r="CF12" s="9">
         <f t="shared" si="3"/>
-        <v>-7.1027786593327348E-5</v>
+        <v>4.7000489408918593E-4</v>
       </c>
       <c r="CG12" s="9">
         <f t="shared" si="3"/>
-        <v>7.102778659333342E-5</v>
+        <v>-4.7000489408918419E-4</v>
       </c>
       <c r="CH12" s="9">
         <f t="shared" si="3"/>
-        <v>-7.1027786593327348E-5</v>
+        <v>4.7000489408918593E-4</v>
       </c>
       <c r="CI12" s="9">
         <f t="shared" si="3"/>
-        <v>7.102778659333342E-5</v>
+        <v>-4.7000489408918419E-4</v>
       </c>
       <c r="CJ12" s="7">
         <f t="shared" si="3"/>
@@ -2378,28 +2378,34 @@
       </c>
       <c r="CL12" s="7">
         <f t="shared" si="3"/>
-        <v>-1.870188268387969E-3</v>
+        <v>-1.6778065799174713E-3</v>
       </c>
       <c r="CM12" s="9">
         <f t="shared" si="3"/>
-        <v>-7.5590580314707881E-5</v>
+        <v>-6.0561228170035117E-5</v>
       </c>
       <c r="CN12" s="9">
         <f t="shared" si="3"/>
-        <v>-7.5590580314707881E-5</v>
+        <v>-6.0561228170035117E-5</v>
       </c>
       <c r="CO12" s="9">
         <f t="shared" si="3"/>
-        <v>-9.7596362097852538E-4</v>
+        <v>4.6308316159725769E-4</v>
       </c>
       <c r="CP12" s="9">
         <f t="shared" si="3"/>
-        <v>9.7596362097853405E-4</v>
+        <v>-4.6308316159725423E-4</v>
       </c>
     </row>
     <row r="13" spans="11:94" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="K6:K8"/>
     <mergeCell ref="BZ7:CP7"/>
     <mergeCell ref="AR6:CP6"/>
     <mergeCell ref="P6:AQ6"/>
@@ -2409,12 +2415,6 @@
     <mergeCell ref="AD7:AJ7"/>
     <mergeCell ref="AR7:BH7"/>
     <mergeCell ref="BI7:BY7"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="M6:M8"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="O6:O8"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="K9:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added previous weight on node and weights
</commit_message>
<xml_diff>
--- a/helper ANN/MLP/simplified.weather.numeric.xlsx
+++ b/helper ANN/MLP/simplified.weather.numeric.xlsx
@@ -334,12 +334,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -363,6 +357,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K1:CP13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="BW1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BR9" sqref="BR9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,211 +758,211 @@
     </row>
     <row r="5" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="M6" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="N6" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="24" t="s">
+      <c r="P6" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="25"/>
-      <c r="AE6" s="25"/>
-      <c r="AF6" s="25"/>
-      <c r="AG6" s="25"/>
-      <c r="AH6" s="25"/>
-      <c r="AI6" s="25"/>
-      <c r="AJ6" s="25"/>
-      <c r="AK6" s="25"/>
-      <c r="AL6" s="25"/>
-      <c r="AM6" s="25"/>
-      <c r="AN6" s="25"/>
-      <c r="AO6" s="25"/>
-      <c r="AP6" s="25"/>
-      <c r="AQ6" s="26"/>
-      <c r="AR6" s="23" t="s">
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="23"/>
+      <c r="AB6" s="23"/>
+      <c r="AC6" s="23"/>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="23"/>
+      <c r="AG6" s="23"/>
+      <c r="AH6" s="23"/>
+      <c r="AI6" s="23"/>
+      <c r="AJ6" s="23"/>
+      <c r="AK6" s="23"/>
+      <c r="AL6" s="23"/>
+      <c r="AM6" s="23"/>
+      <c r="AN6" s="23"/>
+      <c r="AO6" s="23"/>
+      <c r="AP6" s="23"/>
+      <c r="AQ6" s="24"/>
+      <c r="AR6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="AS6" s="23"/>
-      <c r="AT6" s="23"/>
-      <c r="AU6" s="23"/>
-      <c r="AV6" s="23"/>
-      <c r="AW6" s="23"/>
-      <c r="AX6" s="23"/>
-      <c r="AY6" s="23"/>
-      <c r="AZ6" s="23"/>
-      <c r="BA6" s="23"/>
-      <c r="BB6" s="23"/>
-      <c r="BC6" s="23"/>
-      <c r="BD6" s="23"/>
-      <c r="BE6" s="23"/>
-      <c r="BF6" s="23"/>
-      <c r="BG6" s="23"/>
-      <c r="BH6" s="23"/>
-      <c r="BI6" s="23"/>
-      <c r="BJ6" s="23"/>
-      <c r="BK6" s="23"/>
-      <c r="BL6" s="23"/>
-      <c r="BM6" s="23"/>
-      <c r="BN6" s="23"/>
-      <c r="BO6" s="23"/>
-      <c r="BP6" s="23"/>
-      <c r="BQ6" s="23"/>
-      <c r="BR6" s="23"/>
-      <c r="BS6" s="23"/>
-      <c r="BT6" s="23"/>
-      <c r="BU6" s="23"/>
-      <c r="BV6" s="23"/>
-      <c r="BW6" s="23"/>
-      <c r="BX6" s="23"/>
-      <c r="BY6" s="23"/>
-      <c r="BZ6" s="23"/>
-      <c r="CA6" s="23"/>
-      <c r="CB6" s="23"/>
-      <c r="CC6" s="23"/>
-      <c r="CD6" s="23"/>
-      <c r="CE6" s="23"/>
-      <c r="CF6" s="23"/>
-      <c r="CG6" s="23"/>
-      <c r="CH6" s="23"/>
-      <c r="CI6" s="23"/>
-      <c r="CJ6" s="23"/>
-      <c r="CK6" s="23"/>
-      <c r="CL6" s="23"/>
-      <c r="CM6" s="23"/>
-      <c r="CN6" s="23"/>
-      <c r="CO6" s="23"/>
-      <c r="CP6" s="23"/>
+      <c r="AS6" s="21"/>
+      <c r="AT6" s="21"/>
+      <c r="AU6" s="21"/>
+      <c r="AV6" s="21"/>
+      <c r="AW6" s="21"/>
+      <c r="AX6" s="21"/>
+      <c r="AY6" s="21"/>
+      <c r="AZ6" s="21"/>
+      <c r="BA6" s="21"/>
+      <c r="BB6" s="21"/>
+      <c r="BC6" s="21"/>
+      <c r="BD6" s="21"/>
+      <c r="BE6" s="21"/>
+      <c r="BF6" s="21"/>
+      <c r="BG6" s="21"/>
+      <c r="BH6" s="21"/>
+      <c r="BI6" s="21"/>
+      <c r="BJ6" s="21"/>
+      <c r="BK6" s="21"/>
+      <c r="BL6" s="21"/>
+      <c r="BM6" s="21"/>
+      <c r="BN6" s="21"/>
+      <c r="BO6" s="21"/>
+      <c r="BP6" s="21"/>
+      <c r="BQ6" s="21"/>
+      <c r="BR6" s="21"/>
+      <c r="BS6" s="21"/>
+      <c r="BT6" s="21"/>
+      <c r="BU6" s="21"/>
+      <c r="BV6" s="21"/>
+      <c r="BW6" s="21"/>
+      <c r="BX6" s="21"/>
+      <c r="BY6" s="21"/>
+      <c r="BZ6" s="21"/>
+      <c r="CA6" s="21"/>
+      <c r="CB6" s="21"/>
+      <c r="CC6" s="21"/>
+      <c r="CD6" s="21"/>
+      <c r="CE6" s="21"/>
+      <c r="CF6" s="21"/>
+      <c r="CG6" s="21"/>
+      <c r="CH6" s="21"/>
+      <c r="CI6" s="21"/>
+      <c r="CJ6" s="21"/>
+      <c r="CK6" s="21"/>
+      <c r="CL6" s="21"/>
+      <c r="CM6" s="21"/>
+      <c r="CN6" s="21"/>
+      <c r="CO6" s="21"/>
+      <c r="CP6" s="21"/>
     </row>
     <row r="7" spans="11:94" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="22" t="s">
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22" t="s">
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="22"/>
-      <c r="Z7" s="22"/>
-      <c r="AA7" s="22"/>
-      <c r="AB7" s="22"/>
-      <c r="AC7" s="22"/>
-      <c r="AD7" s="22" t="s">
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="AE7" s="22"/>
-      <c r="AF7" s="22"/>
-      <c r="AG7" s="22"/>
-      <c r="AH7" s="22"/>
-      <c r="AI7" s="22"/>
-      <c r="AJ7" s="22"/>
-      <c r="AK7" s="27" t="s">
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" s="20"/>
+      <c r="AK7" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="AL7" s="28"/>
-      <c r="AM7" s="28"/>
-      <c r="AN7" s="28"/>
-      <c r="AO7" s="28"/>
-      <c r="AP7" s="28"/>
-      <c r="AQ7" s="29"/>
-      <c r="AR7" s="22" t="s">
+      <c r="AL7" s="26"/>
+      <c r="AM7" s="26"/>
+      <c r="AN7" s="26"/>
+      <c r="AO7" s="26"/>
+      <c r="AP7" s="26"/>
+      <c r="AQ7" s="27"/>
+      <c r="AR7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AS7" s="22"/>
-      <c r="AT7" s="22"/>
-      <c r="AU7" s="22"/>
-      <c r="AV7" s="22"/>
-      <c r="AW7" s="22"/>
-      <c r="AX7" s="22"/>
-      <c r="AY7" s="22"/>
-      <c r="AZ7" s="22"/>
-      <c r="BA7" s="22"/>
-      <c r="BB7" s="22"/>
-      <c r="BC7" s="22"/>
-      <c r="BD7" s="22"/>
-      <c r="BE7" s="22"/>
-      <c r="BF7" s="22"/>
-      <c r="BG7" s="22"/>
-      <c r="BH7" s="22"/>
-      <c r="BI7" s="22" t="s">
+      <c r="AS7" s="20"/>
+      <c r="AT7" s="20"/>
+      <c r="AU7" s="20"/>
+      <c r="AV7" s="20"/>
+      <c r="AW7" s="20"/>
+      <c r="AX7" s="20"/>
+      <c r="AY7" s="20"/>
+      <c r="AZ7" s="20"/>
+      <c r="BA7" s="20"/>
+      <c r="BB7" s="20"/>
+      <c r="BC7" s="20"/>
+      <c r="BD7" s="20"/>
+      <c r="BE7" s="20"/>
+      <c r="BF7" s="20"/>
+      <c r="BG7" s="20"/>
+      <c r="BH7" s="20"/>
+      <c r="BI7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="BJ7" s="22"/>
-      <c r="BK7" s="22"/>
-      <c r="BL7" s="22"/>
-      <c r="BM7" s="22"/>
-      <c r="BN7" s="22"/>
-      <c r="BO7" s="22"/>
-      <c r="BP7" s="22"/>
-      <c r="BQ7" s="22"/>
-      <c r="BR7" s="22"/>
-      <c r="BS7" s="22"/>
-      <c r="BT7" s="22"/>
-      <c r="BU7" s="22"/>
-      <c r="BV7" s="22"/>
-      <c r="BW7" s="22"/>
-      <c r="BX7" s="22"/>
-      <c r="BY7" s="22"/>
-      <c r="BZ7" s="22" t="s">
+      <c r="BJ7" s="20"/>
+      <c r="BK7" s="20"/>
+      <c r="BL7" s="20"/>
+      <c r="BM7" s="20"/>
+      <c r="BN7" s="20"/>
+      <c r="BO7" s="20"/>
+      <c r="BP7" s="20"/>
+      <c r="BQ7" s="20"/>
+      <c r="BR7" s="20"/>
+      <c r="BS7" s="20"/>
+      <c r="BT7" s="20"/>
+      <c r="BU7" s="20"/>
+      <c r="BV7" s="20"/>
+      <c r="BW7" s="20"/>
+      <c r="BX7" s="20"/>
+      <c r="BY7" s="20"/>
+      <c r="BZ7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="CA7" s="22"/>
-      <c r="CB7" s="22"/>
-      <c r="CC7" s="22"/>
-      <c r="CD7" s="22"/>
-      <c r="CE7" s="22"/>
-      <c r="CF7" s="22"/>
-      <c r="CG7" s="22"/>
-      <c r="CH7" s="22"/>
-      <c r="CI7" s="22"/>
-      <c r="CJ7" s="22"/>
-      <c r="CK7" s="22"/>
-      <c r="CL7" s="22"/>
-      <c r="CM7" s="22"/>
-      <c r="CN7" s="22"/>
-      <c r="CO7" s="22"/>
-      <c r="CP7" s="22"/>
+      <c r="CA7" s="20"/>
+      <c r="CB7" s="20"/>
+      <c r="CC7" s="20"/>
+      <c r="CD7" s="20"/>
+      <c r="CE7" s="20"/>
+      <c r="CF7" s="20"/>
+      <c r="CG7" s="20"/>
+      <c r="CH7" s="20"/>
+      <c r="CI7" s="20"/>
+      <c r="CJ7" s="20"/>
+      <c r="CK7" s="20"/>
+      <c r="CL7" s="20"/>
+      <c r="CM7" s="20"/>
+      <c r="CN7" s="20"/>
+      <c r="CO7" s="20"/>
+      <c r="CP7" s="20"/>
     </row>
     <row r="8" spans="11:94" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
       <c r="P8" s="2">
         <v>0</v>
       </c>
@@ -1202,7 +1202,7 @@
       </c>
     </row>
     <row r="9" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K9" s="20">
+      <c r="K9" s="28">
         <v>1</v>
       </c>
       <c r="L9" s="10">
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="10" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K10" s="20"/>
+      <c r="K10" s="28"/>
       <c r="L10" s="11">
         <v>80</v>
       </c>
@@ -1788,7 +1788,7 @@
       </c>
     </row>
     <row r="11" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K11" s="20"/>
+      <c r="K11" s="28"/>
       <c r="L11" s="11">
         <v>83</v>
       </c>
@@ -2093,7 +2093,7 @@
       </c>
     </row>
     <row r="12" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K12" s="20"/>
+      <c r="K12" s="28"/>
       <c r="L12" s="6">
         <v>70</v>
       </c>
@@ -2400,6 +2400,12 @@
     <row r="13" spans="11:94" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="K6:K8"/>
     <mergeCell ref="BZ7:CP7"/>
     <mergeCell ref="AR6:CP6"/>
     <mergeCell ref="P6:AQ6"/>
@@ -2409,12 +2415,6 @@
     <mergeCell ref="AD7:AJ7"/>
     <mergeCell ref="AR7:BH7"/>
     <mergeCell ref="BI7:BY7"/>
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="M6:M8"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="O6:O8"/>
-    <mergeCell ref="K6:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
update simplified.weather.nominal.arff test set todo: error epoch, looping until num iterations | epoch threshold
</commit_message>
<xml_diff>
--- a/helper ANN/MLP/simplified.weather.numeric.xlsx
+++ b/helper ANN/MLP/simplified.weather.numeric.xlsx
@@ -334,6 +334,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,12 +363,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -394,7 +394,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>485046</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -716,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="K1:CP13"/>
+  <dimension ref="K1:CP17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BW1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BR9" sqref="BR9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BJ14" sqref="BJ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,211 +758,211 @@
     </row>
     <row r="5" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K6" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" s="29" t="s">
+      <c r="K6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="M6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="29" t="s">
+      <c r="N6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="29" t="s">
+      <c r="O6" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="22" t="s">
+      <c r="P6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="23"/>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="23"/>
-      <c r="AF6" s="23"/>
-      <c r="AG6" s="23"/>
-      <c r="AH6" s="23"/>
-      <c r="AI6" s="23"/>
-      <c r="AJ6" s="23"/>
-      <c r="AK6" s="23"/>
-      <c r="AL6" s="23"/>
-      <c r="AM6" s="23"/>
-      <c r="AN6" s="23"/>
-      <c r="AO6" s="23"/>
-      <c r="AP6" s="23"/>
-      <c r="AQ6" s="24"/>
-      <c r="AR6" s="21" t="s">
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="25"/>
+      <c r="AD6" s="25"/>
+      <c r="AE6" s="25"/>
+      <c r="AF6" s="25"/>
+      <c r="AG6" s="25"/>
+      <c r="AH6" s="25"/>
+      <c r="AI6" s="25"/>
+      <c r="AJ6" s="25"/>
+      <c r="AK6" s="25"/>
+      <c r="AL6" s="25"/>
+      <c r="AM6" s="25"/>
+      <c r="AN6" s="25"/>
+      <c r="AO6" s="25"/>
+      <c r="AP6" s="25"/>
+      <c r="AQ6" s="26"/>
+      <c r="AR6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="AS6" s="21"/>
-      <c r="AT6" s="21"/>
-      <c r="AU6" s="21"/>
-      <c r="AV6" s="21"/>
-      <c r="AW6" s="21"/>
-      <c r="AX6" s="21"/>
-      <c r="AY6" s="21"/>
-      <c r="AZ6" s="21"/>
-      <c r="BA6" s="21"/>
-      <c r="BB6" s="21"/>
-      <c r="BC6" s="21"/>
-      <c r="BD6" s="21"/>
-      <c r="BE6" s="21"/>
-      <c r="BF6" s="21"/>
-      <c r="BG6" s="21"/>
-      <c r="BH6" s="21"/>
-      <c r="BI6" s="21"/>
-      <c r="BJ6" s="21"/>
-      <c r="BK6" s="21"/>
-      <c r="BL6" s="21"/>
-      <c r="BM6" s="21"/>
-      <c r="BN6" s="21"/>
-      <c r="BO6" s="21"/>
-      <c r="BP6" s="21"/>
-      <c r="BQ6" s="21"/>
-      <c r="BR6" s="21"/>
-      <c r="BS6" s="21"/>
-      <c r="BT6" s="21"/>
-      <c r="BU6" s="21"/>
-      <c r="BV6" s="21"/>
-      <c r="BW6" s="21"/>
-      <c r="BX6" s="21"/>
-      <c r="BY6" s="21"/>
-      <c r="BZ6" s="21"/>
-      <c r="CA6" s="21"/>
-      <c r="CB6" s="21"/>
-      <c r="CC6" s="21"/>
-      <c r="CD6" s="21"/>
-      <c r="CE6" s="21"/>
-      <c r="CF6" s="21"/>
-      <c r="CG6" s="21"/>
-      <c r="CH6" s="21"/>
-      <c r="CI6" s="21"/>
-      <c r="CJ6" s="21"/>
-      <c r="CK6" s="21"/>
-      <c r="CL6" s="21"/>
-      <c r="CM6" s="21"/>
-      <c r="CN6" s="21"/>
-      <c r="CO6" s="21"/>
-      <c r="CP6" s="21"/>
+      <c r="AS6" s="23"/>
+      <c r="AT6" s="23"/>
+      <c r="AU6" s="23"/>
+      <c r="AV6" s="23"/>
+      <c r="AW6" s="23"/>
+      <c r="AX6" s="23"/>
+      <c r="AY6" s="23"/>
+      <c r="AZ6" s="23"/>
+      <c r="BA6" s="23"/>
+      <c r="BB6" s="23"/>
+      <c r="BC6" s="23"/>
+      <c r="BD6" s="23"/>
+      <c r="BE6" s="23"/>
+      <c r="BF6" s="23"/>
+      <c r="BG6" s="23"/>
+      <c r="BH6" s="23"/>
+      <c r="BI6" s="23"/>
+      <c r="BJ6" s="23"/>
+      <c r="BK6" s="23"/>
+      <c r="BL6" s="23"/>
+      <c r="BM6" s="23"/>
+      <c r="BN6" s="23"/>
+      <c r="BO6" s="23"/>
+      <c r="BP6" s="23"/>
+      <c r="BQ6" s="23"/>
+      <c r="BR6" s="23"/>
+      <c r="BS6" s="23"/>
+      <c r="BT6" s="23"/>
+      <c r="BU6" s="23"/>
+      <c r="BV6" s="23"/>
+      <c r="BW6" s="23"/>
+      <c r="BX6" s="23"/>
+      <c r="BY6" s="23"/>
+      <c r="BZ6" s="23"/>
+      <c r="CA6" s="23"/>
+      <c r="CB6" s="23"/>
+      <c r="CC6" s="23"/>
+      <c r="CD6" s="23"/>
+      <c r="CE6" s="23"/>
+      <c r="CF6" s="23"/>
+      <c r="CG6" s="23"/>
+      <c r="CH6" s="23"/>
+      <c r="CI6" s="23"/>
+      <c r="CJ6" s="23"/>
+      <c r="CK6" s="23"/>
+      <c r="CL6" s="23"/>
+      <c r="CM6" s="23"/>
+      <c r="CN6" s="23"/>
+      <c r="CO6" s="23"/>
+      <c r="CP6" s="23"/>
     </row>
     <row r="7" spans="11:94" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="20" t="s">
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="20" t="s">
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="20"/>
-      <c r="Z7" s="20"/>
-      <c r="AA7" s="20"/>
-      <c r="AB7" s="20"/>
-      <c r="AC7" s="20"/>
-      <c r="AD7" s="20" t="s">
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
+      <c r="AA7" s="22"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
+      <c r="AD7" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="AE7" s="20"/>
-      <c r="AF7" s="20"/>
-      <c r="AG7" s="20"/>
-      <c r="AH7" s="20"/>
-      <c r="AI7" s="20"/>
-      <c r="AJ7" s="20"/>
-      <c r="AK7" s="25" t="s">
+      <c r="AE7" s="22"/>
+      <c r="AF7" s="22"/>
+      <c r="AG7" s="22"/>
+      <c r="AH7" s="22"/>
+      <c r="AI7" s="22"/>
+      <c r="AJ7" s="22"/>
+      <c r="AK7" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="AL7" s="26"/>
-      <c r="AM7" s="26"/>
-      <c r="AN7" s="26"/>
-      <c r="AO7" s="26"/>
-      <c r="AP7" s="26"/>
-      <c r="AQ7" s="27"/>
-      <c r="AR7" s="20" t="s">
+      <c r="AL7" s="28"/>
+      <c r="AM7" s="28"/>
+      <c r="AN7" s="28"/>
+      <c r="AO7" s="28"/>
+      <c r="AP7" s="28"/>
+      <c r="AQ7" s="29"/>
+      <c r="AR7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="AS7" s="20"/>
-      <c r="AT7" s="20"/>
-      <c r="AU7" s="20"/>
-      <c r="AV7" s="20"/>
-      <c r="AW7" s="20"/>
-      <c r="AX7" s="20"/>
-      <c r="AY7" s="20"/>
-      <c r="AZ7" s="20"/>
-      <c r="BA7" s="20"/>
-      <c r="BB7" s="20"/>
-      <c r="BC7" s="20"/>
-      <c r="BD7" s="20"/>
-      <c r="BE7" s="20"/>
-      <c r="BF7" s="20"/>
-      <c r="BG7" s="20"/>
-      <c r="BH7" s="20"/>
-      <c r="BI7" s="20" t="s">
+      <c r="AS7" s="22"/>
+      <c r="AT7" s="22"/>
+      <c r="AU7" s="22"/>
+      <c r="AV7" s="22"/>
+      <c r="AW7" s="22"/>
+      <c r="AX7" s="22"/>
+      <c r="AY7" s="22"/>
+      <c r="AZ7" s="22"/>
+      <c r="BA7" s="22"/>
+      <c r="BB7" s="22"/>
+      <c r="BC7" s="22"/>
+      <c r="BD7" s="22"/>
+      <c r="BE7" s="22"/>
+      <c r="BF7" s="22"/>
+      <c r="BG7" s="22"/>
+      <c r="BH7" s="22"/>
+      <c r="BI7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="BJ7" s="20"/>
-      <c r="BK7" s="20"/>
-      <c r="BL7" s="20"/>
-      <c r="BM7" s="20"/>
-      <c r="BN7" s="20"/>
-      <c r="BO7" s="20"/>
-      <c r="BP7" s="20"/>
-      <c r="BQ7" s="20"/>
-      <c r="BR7" s="20"/>
-      <c r="BS7" s="20"/>
-      <c r="BT7" s="20"/>
-      <c r="BU7" s="20"/>
-      <c r="BV7" s="20"/>
-      <c r="BW7" s="20"/>
-      <c r="BX7" s="20"/>
-      <c r="BY7" s="20"/>
-      <c r="BZ7" s="20" t="s">
+      <c r="BJ7" s="22"/>
+      <c r="BK7" s="22"/>
+      <c r="BL7" s="22"/>
+      <c r="BM7" s="22"/>
+      <c r="BN7" s="22"/>
+      <c r="BO7" s="22"/>
+      <c r="BP7" s="22"/>
+      <c r="BQ7" s="22"/>
+      <c r="BR7" s="22"/>
+      <c r="BS7" s="22"/>
+      <c r="BT7" s="22"/>
+      <c r="BU7" s="22"/>
+      <c r="BV7" s="22"/>
+      <c r="BW7" s="22"/>
+      <c r="BX7" s="22"/>
+      <c r="BY7" s="22"/>
+      <c r="BZ7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="CA7" s="20"/>
-      <c r="CB7" s="20"/>
-      <c r="CC7" s="20"/>
-      <c r="CD7" s="20"/>
-      <c r="CE7" s="20"/>
-      <c r="CF7" s="20"/>
-      <c r="CG7" s="20"/>
-      <c r="CH7" s="20"/>
-      <c r="CI7" s="20"/>
-      <c r="CJ7" s="20"/>
-      <c r="CK7" s="20"/>
-      <c r="CL7" s="20"/>
-      <c r="CM7" s="20"/>
-      <c r="CN7" s="20"/>
-      <c r="CO7" s="20"/>
-      <c r="CP7" s="20"/>
+      <c r="CA7" s="22"/>
+      <c r="CB7" s="22"/>
+      <c r="CC7" s="22"/>
+      <c r="CD7" s="22"/>
+      <c r="CE7" s="22"/>
+      <c r="CF7" s="22"/>
+      <c r="CG7" s="22"/>
+      <c r="CH7" s="22"/>
+      <c r="CI7" s="22"/>
+      <c r="CJ7" s="22"/>
+      <c r="CK7" s="22"/>
+      <c r="CL7" s="22"/>
+      <c r="CM7" s="22"/>
+      <c r="CN7" s="22"/>
+      <c r="CO7" s="22"/>
+      <c r="CP7" s="22"/>
     </row>
     <row r="8" spans="11:94" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
       <c r="P8" s="2">
         <v>0</v>
       </c>
@@ -1202,7 +1202,7 @@
       </c>
     </row>
     <row r="9" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K9" s="28">
+      <c r="K9" s="20">
         <v>1</v>
       </c>
       <c r="L9" s="10">
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="10" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K10" s="28"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="11">
         <v>80</v>
       </c>
@@ -1520,11 +1520,11 @@
         <v>80</v>
       </c>
       <c r="X10" s="11">
-        <f t="shared" ref="X10:X12" si="9">M10</f>
+        <f t="shared" ref="X10:X13" si="9">M10</f>
         <v>90</v>
       </c>
       <c r="Y10" s="11">
-        <f t="shared" ref="Y10:Y12" si="10">N10</f>
+        <f t="shared" ref="Y10:Y13" si="10">N10</f>
         <v>0</v>
       </c>
       <c r="Z10" s="8">
@@ -1532,15 +1532,15 @@
         <v>0.99999996254028922</v>
       </c>
       <c r="AA10" s="8">
-        <f t="shared" ref="AA10:AA12" si="12">1/(1+EXP(-T10))</f>
+        <f t="shared" ref="AA10:AA13" si="12">1/(1+EXP(-T10))</f>
         <v>0.99999996254028922</v>
       </c>
       <c r="AB10" s="8">
-        <f t="shared" ref="AB10:AB12" si="13">1/(1+EXP(-U10))</f>
+        <f t="shared" ref="AB10:AB13" si="13">1/(1+EXP(-U10))</f>
         <v>0.5641130663041356</v>
       </c>
       <c r="AC10" s="8">
-        <f t="shared" ref="AC10:AC12" si="14">1/(1+EXP(-V10))</f>
+        <f t="shared" ref="AC10:AC13" si="14">1/(1+EXP(-V10))</f>
         <v>0.58205359154975622</v>
       </c>
       <c r="AD10" s="15"/>
@@ -1587,67 +1587,67 @@
         <v>9.9999998951400493E-2</v>
       </c>
       <c r="AS10" s="8">
-        <f t="shared" ref="AS10:AS12" si="22">CA9</f>
+        <f t="shared" ref="AS10:AS16" si="22">CA9</f>
         <v>9.9999998951400493E-2</v>
       </c>
       <c r="AT10" s="8">
-        <f t="shared" ref="AT10:AT12" si="23">CB9</f>
+        <f t="shared" ref="AT10:AT16" si="23">CB9</f>
         <v>9.9999998951400493E-2</v>
       </c>
       <c r="AU10" s="8">
-        <f t="shared" ref="AU10:AU12" si="24">CC9</f>
+        <f t="shared" ref="AU10:AU16" si="24">CC9</f>
         <v>9.9999998951400493E-2</v>
       </c>
       <c r="AV10" s="8">
-        <f t="shared" ref="AV10:AV12" si="25">CD9</f>
+        <f t="shared" ref="AV10:AV16" si="25">CD9</f>
         <v>9.999999998766354E-2</v>
       </c>
       <c r="AW10" s="8">
-        <f t="shared" ref="AW10:AW12" si="26">CE9</f>
+        <f t="shared" ref="AW10:AW16" si="26">CE9</f>
         <v>9.999999998766354E-2</v>
       </c>
       <c r="AX10" s="8">
-        <f t="shared" ref="AX10:AX12" si="27">CF9</f>
+        <f t="shared" ref="AX10:AX16" si="27">CF9</f>
         <v>8.5957275719999213E-2</v>
       </c>
       <c r="AY10" s="8">
-        <f t="shared" ref="AY10:AY12" si="28">CG9</f>
+        <f t="shared" ref="AY10:AY16" si="28">CG9</f>
         <v>0.11040310608515669</v>
       </c>
       <c r="AZ10" s="8">
-        <f t="shared" ref="AZ10:AZ12" si="29">CH9</f>
+        <f t="shared" ref="AZ10:AZ16" si="29">CH9</f>
         <v>8.5957275719999213E-2</v>
       </c>
       <c r="BA10" s="8">
-        <f t="shared" ref="BA10:BA12" si="30">CI9</f>
+        <f t="shared" ref="BA10:BA16" si="30">CI9</f>
         <v>0.11040310608515669</v>
       </c>
       <c r="BB10" s="5">
-        <f t="shared" ref="BB10:BB12" si="31">CJ9</f>
+        <f t="shared" ref="BB10:BB16" si="31">CJ9</f>
         <v>0.1</v>
       </c>
       <c r="BC10" s="5">
-        <f t="shared" ref="BC10:BC12" si="32">CK9</f>
+        <f t="shared" ref="BC10:BC16" si="32">CK9</f>
         <v>0.1</v>
       </c>
       <c r="BD10" s="5">
-        <f t="shared" ref="BD10:BD12" si="33">CL9</f>
+        <f t="shared" ref="BD10:BD16" si="33">CL9</f>
         <v>0.1</v>
       </c>
       <c r="BE10" s="8">
-        <f t="shared" ref="BE10:BE12" si="34">CM9</f>
+        <f t="shared" ref="BE10:BE16" si="34">CM9</f>
         <v>9.999999998766354E-2</v>
       </c>
       <c r="BF10" s="8">
-        <f t="shared" ref="BF10:BF12" si="35">CN9</f>
+        <f t="shared" ref="BF10:BF16" si="35">CN9</f>
         <v>9.999999998766354E-2</v>
       </c>
       <c r="BG10" s="8">
-        <f t="shared" ref="BG10:BG12" si="36">CO9</f>
+        <f t="shared" ref="BG10:BG16" si="36">CO9</f>
         <v>8.5957275244021858E-2</v>
       </c>
       <c r="BH10" s="8">
-        <f t="shared" ref="BH10:BH12" si="37">CP9</f>
+        <f t="shared" ref="BH10:BH16" si="37">CP9</f>
         <v>0.11040310643776938</v>
       </c>
       <c r="BI10" s="8">
@@ -1788,7 +1788,7 @@
       </c>
     </row>
     <row r="11" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K11" s="28"/>
+      <c r="K11" s="20"/>
       <c r="L11" s="11">
         <v>83</v>
       </c>
@@ -2093,7 +2093,7 @@
       </c>
     </row>
     <row r="12" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K12" s="28"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="6">
         <v>70</v>
       </c>
@@ -2397,15 +2397,1223 @@
         <v>9.3002775531662252E-2</v>
       </c>
     </row>
-    <row r="13" spans="11:94" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="20">
+        <v>2</v>
+      </c>
+      <c r="L13" s="10">
+        <v>85</v>
+      </c>
+      <c r="M13" s="10">
+        <v>85</v>
+      </c>
+      <c r="N13" s="10">
+        <v>1</v>
+      </c>
+      <c r="O13" s="10">
+        <v>1</v>
+      </c>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="4">
+        <f>AR13*W13+AT13*X13+AV13*Y13+$L$4*BE13</f>
+        <v>17.199998721407564</v>
+      </c>
+      <c r="T13" s="4">
+        <f>AS13*W13+AU13*X13+AW13*Y13+$L$4*BF13</f>
+        <v>17.199998721407564</v>
+      </c>
+      <c r="U13" s="4">
+        <f>AX13*Z13+AZ13*AA13+BG13*$L$4</f>
+        <v>0.27602317655985731</v>
+      </c>
+      <c r="V13" s="4">
+        <f>AY13*Z13+BA13*AA13+BH13*$L$4</f>
+        <v>0.27900832126754449</v>
+      </c>
+      <c r="W13" s="10">
+        <f>L13</f>
+        <v>85</v>
+      </c>
+      <c r="X13" s="10">
+        <f t="shared" si="9"/>
+        <v>85</v>
+      </c>
+      <c r="Y13" s="10">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="Z13" s="4">
+        <f>1/(1+EXP(-S13))</f>
+        <v>0.99999996610501451</v>
+      </c>
+      <c r="AA13" s="4">
+        <f t="shared" si="12"/>
+        <v>0.99999996610501451</v>
+      </c>
+      <c r="AB13" s="4">
+        <f t="shared" si="13"/>
+        <v>0.56857098425098596</v>
+      </c>
+      <c r="AC13" s="4">
+        <f t="shared" si="14"/>
+        <v>0.56930308393725881</v>
+      </c>
+      <c r="AD13" s="14"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="14"/>
+      <c r="AG13" s="14"/>
+      <c r="AH13" s="14"/>
+      <c r="AI13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="4">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="4">
+        <f>W13*(1-W13)*(AR13*AN13+AS13*AO13)</f>
+        <v>1.457211122916481E-7</v>
+      </c>
+      <c r="AL13" s="4">
+        <f>X13*(1-X13)*(AT13*AN13+AU13*AO13)</f>
+        <v>1.4572111080630571E-7</v>
+      </c>
+      <c r="AM13" s="4">
+        <f>Y13*(1-Y13)*(AV13*AN13+AW13*AO13)</f>
+        <v>0</v>
+      </c>
+      <c r="AN13" s="4">
+        <f>Z13*(1-Z13)*(AX13*AP13+AY13*AQ13)</f>
+        <v>-1.0204560399674057E-10</v>
+      </c>
+      <c r="AO13" s="4">
+        <f>AA13*(1-AA13)*(AZ13*AP13+BA13*AQ13)</f>
+        <v>-1.0204560399674057E-10</v>
+      </c>
+      <c r="AP13" s="4">
+        <f>AB13*(1-AB13)*(AI13-AB13)</f>
+        <v>-0.1394693367337933</v>
+      </c>
+      <c r="AQ13" s="4">
+        <f>AC13*(1-AC13)*(AJ13-AC13)</f>
+        <v>0.10560562728478877</v>
+      </c>
+      <c r="AR13" s="4">
+        <f>BZ12</f>
+        <v>9.9999992989556169E-2</v>
+      </c>
+      <c r="AS13" s="4">
+        <f t="shared" si="22"/>
+        <v>9.9999992989556169E-2</v>
+      </c>
+      <c r="AT13" s="4">
+        <f t="shared" si="23"/>
+        <v>9.999999197025139E-2</v>
+      </c>
+      <c r="AU13" s="4">
+        <f t="shared" si="24"/>
+        <v>9.999999197025139E-2</v>
+      </c>
+      <c r="AV13" s="4">
+        <f t="shared" si="25"/>
+        <v>9.9999999913410284E-2</v>
+      </c>
+      <c r="AW13" s="4">
+        <f t="shared" si="26"/>
+        <v>9.9999999913410284E-2</v>
+      </c>
+      <c r="AX13" s="4">
+        <f t="shared" si="27"/>
+        <v>9.2007727632897815E-2</v>
+      </c>
+      <c r="AY13" s="4">
+        <f t="shared" si="28"/>
+        <v>9.3002776020268851E-2</v>
+      </c>
+      <c r="AZ13" s="4">
+        <f t="shared" si="29"/>
+        <v>9.2007727632897815E-2</v>
+      </c>
+      <c r="BA13" s="4">
+        <f t="shared" si="30"/>
+        <v>9.3002776020268851E-2</v>
+      </c>
+      <c r="BB13" s="3">
+        <f t="shared" si="31"/>
+        <v>0.1</v>
+      </c>
+      <c r="BC13" s="3">
+        <f t="shared" si="32"/>
+        <v>0.1</v>
+      </c>
+      <c r="BD13" s="3">
+        <f t="shared" si="33"/>
+        <v>0.11508915090845562</v>
+      </c>
+      <c r="BE13" s="4">
+        <f t="shared" si="34"/>
+        <v>9.9999999910507509E-2</v>
+      </c>
+      <c r="BF13" s="4">
+        <f t="shared" si="35"/>
+        <v>9.9999999910507509E-2</v>
+      </c>
+      <c r="BG13" s="4">
+        <f t="shared" si="36"/>
+        <v>9.2007727531262878E-2</v>
+      </c>
+      <c r="BH13" s="4">
+        <f t="shared" si="37"/>
+        <v>9.3002775531662252E-2</v>
+      </c>
+      <c r="BI13" s="4">
+        <f>$L$2*AN13*W13</f>
+        <v>-8.6738763397229483E-10</v>
+      </c>
+      <c r="BJ13" s="4">
+        <f>$L$2*AO13*W13</f>
+        <v>-8.6738763397229483E-10</v>
+      </c>
+      <c r="BK13" s="4">
+        <f>$L$2*AN13*X13</f>
+        <v>-8.6738763397229483E-10</v>
+      </c>
+      <c r="BL13" s="4">
+        <f>$L$2*AO13*X13</f>
+        <v>-8.6738763397229483E-10</v>
+      </c>
+      <c r="BM13" s="4">
+        <f>$L$2*AN13*Y13</f>
+        <v>-1.0204560399674057E-11</v>
+      </c>
+      <c r="BN13" s="4">
+        <f>$L$2*AO13*Y13</f>
+        <v>-1.0204560399674057E-11</v>
+      </c>
+      <c r="BO13" s="4">
+        <f>$L$2*AP13*Z13</f>
+        <v>-1.3946933200648217E-2</v>
+      </c>
+      <c r="BP13" s="4">
+        <f>$L$2*AQ13*Z13</f>
+        <v>1.0560562370528756E-2</v>
+      </c>
+      <c r="BQ13" s="4">
+        <f>$L$2*AP13*AA13</f>
+        <v>-1.3946933200648217E-2</v>
+      </c>
+      <c r="BR13" s="4">
+        <f>$L$2*AQ13*AA13</f>
+        <v>1.0560562370528756E-2</v>
+      </c>
+      <c r="BS13" s="3"/>
+      <c r="BT13" s="3"/>
+      <c r="BU13" s="3"/>
+      <c r="BV13" s="4">
+        <f>$L$2*AN13*$L$4</f>
+        <v>-1.0204560399674057E-11</v>
+      </c>
+      <c r="BW13" s="4">
+        <f>$L$2*AO13*$L$4</f>
+        <v>-1.0204560399674057E-11</v>
+      </c>
+      <c r="BX13" s="4">
+        <f t="shared" ref="BX13" si="60">$L$2*AP13*$L$4</f>
+        <v>-1.3946933673379331E-2</v>
+      </c>
+      <c r="BY13" s="4">
+        <f t="shared" ref="BY13" si="61">$L$2*AQ13*$L$4</f>
+        <v>1.0560562728478877E-2</v>
+      </c>
+      <c r="BZ13" s="4">
+        <f>AR13+BI13</f>
+        <v>9.9999992122168535E-2</v>
+      </c>
+      <c r="CA13" s="4">
+        <f t="shared" ref="CA13:CA16" si="62">AS13+BJ13</f>
+        <v>9.9999992122168535E-2</v>
+      </c>
+      <c r="CB13" s="4">
+        <f t="shared" ref="CB13:CB16" si="63">AT13+BK13</f>
+        <v>9.9999991102863756E-2</v>
+      </c>
+      <c r="CC13" s="4">
+        <f t="shared" ref="CC13:CC16" si="64">AU13+BL13</f>
+        <v>9.9999991102863756E-2</v>
+      </c>
+      <c r="CD13" s="4">
+        <f t="shared" ref="CD13:CD16" si="65">AV13+BM13</f>
+        <v>9.9999999903205725E-2</v>
+      </c>
+      <c r="CE13" s="4">
+        <f t="shared" ref="CE13:CE16" si="66">AW13+BN13</f>
+        <v>9.9999999903205725E-2</v>
+      </c>
+      <c r="CF13" s="4">
+        <f t="shared" ref="CF13:CF16" si="67">AX13+BO13</f>
+        <v>7.80607944322496E-2</v>
+      </c>
+      <c r="CG13" s="4">
+        <f t="shared" ref="CG13:CG16" si="68">AY13+BP13</f>
+        <v>0.10356333839079761</v>
+      </c>
+      <c r="CH13" s="4">
+        <f t="shared" ref="CH13:CH16" si="69">AZ13+BQ13</f>
+        <v>7.80607944322496E-2</v>
+      </c>
+      <c r="CI13" s="4">
+        <f t="shared" ref="CI13:CI16" si="70">BA13+BR13</f>
+        <v>0.10356333839079761</v>
+      </c>
+      <c r="CJ13" s="3">
+        <f t="shared" ref="CJ13:CJ16" si="71">BB13+BS13</f>
+        <v>0.1</v>
+      </c>
+      <c r="CK13" s="3">
+        <f t="shared" ref="CK13:CK16" si="72">BC13+BT13</f>
+        <v>0.1</v>
+      </c>
+      <c r="CL13" s="3">
+        <f t="shared" ref="CL13:CL16" si="73">BD13+BU13</f>
+        <v>0.11508915090845562</v>
+      </c>
+      <c r="CM13" s="4">
+        <f t="shared" ref="CM13:CM16" si="74">BE13+BV13</f>
+        <v>9.9999999900302949E-2</v>
+      </c>
+      <c r="CN13" s="4">
+        <f t="shared" ref="CN13:CN16" si="75">BF13+BW13</f>
+        <v>9.9999999900302949E-2</v>
+      </c>
+      <c r="CO13" s="4">
+        <f t="shared" ref="CO13:CO16" si="76">BG13+BX13</f>
+        <v>7.8060793857883545E-2</v>
+      </c>
+      <c r="CP13" s="4">
+        <f t="shared" ref="CP13:CP16" si="77">BH13+BY13</f>
+        <v>0.10356333826014114</v>
+      </c>
+    </row>
+    <row r="14" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K14" s="20"/>
+      <c r="L14" s="11">
+        <v>80</v>
+      </c>
+      <c r="M14" s="11">
+        <v>90</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0</v>
+      </c>
+      <c r="O14" s="11">
+        <v>1</v>
+      </c>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="8">
+        <f t="shared" ref="S14:S16" si="78">AR14*W14+AT14*X14+AV14*Y14+$L$4*BE14</f>
+        <v>17.099998568931522</v>
+      </c>
+      <c r="T14" s="8">
+        <f t="shared" ref="T14:T16" si="79">AS14*W14+AU14*X14+AW14*Y14+$L$4*BF14</f>
+        <v>17.099998568931522</v>
+      </c>
+      <c r="U14" s="8">
+        <f t="shared" ref="U14:U16" si="80">AX14*Z14+AZ14*AA14+BG14*$L$4</f>
+        <v>0.23418237687410587</v>
+      </c>
+      <c r="V14" s="8">
+        <f t="shared" ref="V14:V16" si="81">AY14*Z14+BA14*AA14+BH14*$L$4</f>
+        <v>0.31069000728282126</v>
+      </c>
+      <c r="W14" s="11">
+        <f t="shared" ref="W14:W16" si="82">L14</f>
+        <v>80</v>
+      </c>
+      <c r="X14" s="11">
+        <f t="shared" ref="X14:X16" si="83">M14</f>
+        <v>90</v>
+      </c>
+      <c r="Y14" s="11">
+        <f t="shared" ref="Y14:Y16" si="84">N14</f>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="8">
+        <f t="shared" ref="Z14:Z16" si="85">1/(1+EXP(-S14))</f>
+        <v>0.99999996254024237</v>
+      </c>
+      <c r="AA14" s="8">
+        <f t="shared" ref="AA14:AA16" si="86">1/(1+EXP(-T14))</f>
+        <v>0.99999996254024237</v>
+      </c>
+      <c r="AB14" s="8">
+        <f t="shared" ref="AB14:AB16" si="87">1/(1+EXP(-U14))</f>
+        <v>0.55827949333161353</v>
+      </c>
+      <c r="AC14" s="8">
+        <f t="shared" ref="AC14:AC16" si="88">1/(1+EXP(-V14))</f>
+        <v>0.57705367514148931</v>
+      </c>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="15"/>
+      <c r="AI14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="8">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="8">
+        <f t="shared" ref="AK14:AK16" si="89">W14*(1-W14)*(AR14*AN14+AS14*AO14)</f>
+        <v>2.6774017578645533E-9</v>
+      </c>
+      <c r="AL14" s="8">
+        <f t="shared" ref="AL14:AL16" si="90">X14*(1-X14)*(AT14*AN14+AU14*AO14)</f>
+        <v>3.393352509793524E-9</v>
+      </c>
+      <c r="AM14" s="8">
+        <f t="shared" ref="AM14:AM16" si="91">Y14*(1-Y14)*(AV14*AN14+AW14*AO14)</f>
+        <v>0</v>
+      </c>
+      <c r="AN14" s="8">
+        <f t="shared" ref="AN14:AN16" si="92">Z14*(1-Z14)*(AX14*AP14+AY14*AQ14)</f>
+        <v>-2.1181977601153226E-12</v>
+      </c>
+      <c r="AO14" s="8">
+        <f t="shared" ref="AO14:AO16" si="93">AA14*(1-AA14)*(AZ14*AP14+BA14*AQ14)</f>
+        <v>-2.1181977601153226E-12</v>
+      </c>
+      <c r="AP14" s="8">
+        <f t="shared" ref="AP14:AP16" si="94">AB14*(1-AB14)*(AI14-AB14)</f>
+        <v>-0.13767367740059799</v>
+      </c>
+      <c r="AQ14" s="8">
+        <f t="shared" ref="AQ14:AQ16" si="95">AC14*(1-AC14)*(AJ14-AC14)</f>
+        <v>0.10322543517363471</v>
+      </c>
+      <c r="AR14" s="8">
+        <f t="shared" ref="AR14:AR16" si="96">BZ13</f>
+        <v>9.9999992122168535E-2</v>
+      </c>
+      <c r="AS14" s="8">
+        <f t="shared" si="22"/>
+        <v>9.9999992122168535E-2</v>
+      </c>
+      <c r="AT14" s="8">
+        <f t="shared" si="23"/>
+        <v>9.9999991102863756E-2</v>
+      </c>
+      <c r="AU14" s="8">
+        <f t="shared" si="24"/>
+        <v>9.9999991102863756E-2</v>
+      </c>
+      <c r="AV14" s="8">
+        <f t="shared" si="25"/>
+        <v>9.9999999903205725E-2</v>
+      </c>
+      <c r="AW14" s="8">
+        <f t="shared" si="26"/>
+        <v>9.9999999903205725E-2</v>
+      </c>
+      <c r="AX14" s="8">
+        <f t="shared" si="27"/>
+        <v>7.80607944322496E-2</v>
+      </c>
+      <c r="AY14" s="8">
+        <f t="shared" si="28"/>
+        <v>0.10356333839079761</v>
+      </c>
+      <c r="AZ14" s="8">
+        <f t="shared" si="29"/>
+        <v>7.80607944322496E-2</v>
+      </c>
+      <c r="BA14" s="8">
+        <f t="shared" si="30"/>
+        <v>0.10356333839079761</v>
+      </c>
+      <c r="BB14" s="5">
+        <f t="shared" si="31"/>
+        <v>0.1</v>
+      </c>
+      <c r="BC14" s="5">
+        <f t="shared" si="32"/>
+        <v>0.1</v>
+      </c>
+      <c r="BD14" s="5">
+        <f t="shared" si="33"/>
+        <v>0.11508915090845562</v>
+      </c>
+      <c r="BE14" s="8">
+        <f t="shared" si="34"/>
+        <v>9.9999999900302949E-2</v>
+      </c>
+      <c r="BF14" s="8">
+        <f t="shared" si="35"/>
+        <v>9.9999999900302949E-2</v>
+      </c>
+      <c r="BG14" s="8">
+        <f>CO13</f>
+        <v>7.8060793857883545E-2</v>
+      </c>
+      <c r="BH14" s="8">
+        <f t="shared" si="37"/>
+        <v>0.10356333826014114</v>
+      </c>
+      <c r="BI14" s="8">
+        <f>$L$2*AN14*W14+$L$3*BI13</f>
+        <v>-1.0368434547815208E-10</v>
+      </c>
+      <c r="BJ14" s="8">
+        <f>$L$2*AO14*W14+$L$3*BJ13</f>
+        <v>-1.0368434547815208E-10</v>
+      </c>
+      <c r="BK14" s="8">
+        <f>$L$2*AN14*X14+BK13*$L$3</f>
+        <v>-1.058025432382674E-10</v>
+      </c>
+      <c r="BL14" s="8">
+        <f>$L$2*AO14*X14+BL13*$L$3</f>
+        <v>-1.058025432382674E-10</v>
+      </c>
+      <c r="BM14" s="8">
+        <f>$L$2*AN14*Y14+BM13*$L$3</f>
+        <v>-1.0204560399674057E-12</v>
+      </c>
+      <c r="BN14" s="8">
+        <f>$L$2*AO14*Y14+BN13*$L$3</f>
+        <v>-1.0204560399674057E-12</v>
+      </c>
+      <c r="BO14" s="8">
+        <f>$L$2*AP14*Z14+BO13*$L$3</f>
+        <v>-1.5162060544402365E-2</v>
+      </c>
+      <c r="BP14" s="8">
+        <f>$L$2*AQ14*Z14+BP13*$L$3</f>
+        <v>1.1378599367736369E-2</v>
+      </c>
+      <c r="BQ14" s="8">
+        <f>$L$2*AP14*AA14+BQ13*$L$3</f>
+        <v>-1.5162060544402365E-2</v>
+      </c>
+      <c r="BR14" s="8">
+        <f>$L$2*AQ14*AA14+BR13*$L$3</f>
+        <v>1.1378599367736369E-2</v>
+      </c>
+      <c r="BS14" s="5">
+        <f t="shared" ref="BS14:BS16" si="97">$L$2*AX14*AG14</f>
+        <v>0</v>
+      </c>
+      <c r="BT14" s="5">
+        <f t="shared" ref="BT14:BT16" si="98">$L$2*AY14*AH14</f>
+        <v>0</v>
+      </c>
+      <c r="BU14" s="5">
+        <f t="shared" ref="BU14:BU16" si="99">$L$2*AZ14*AI14</f>
+        <v>0</v>
+      </c>
+      <c r="BV14" s="8">
+        <f>$L$2*AN14*$L$4+BV13*$L$3</f>
+        <v>-1.232275815978938E-12</v>
+      </c>
+      <c r="BW14" s="8">
+        <f>$L$2*AO14*$L$4+BW13*$L$3</f>
+        <v>-1.232275815978938E-12</v>
+      </c>
+      <c r="BX14" s="8">
+        <f>$L$2*AP14*$L$4+BX13*$L$3</f>
+        <v>-1.5162061107397734E-2</v>
+      </c>
+      <c r="BY14" s="8">
+        <f>$L$2*AQ14*$L$4+BY13*$L$3</f>
+        <v>1.137859979021136E-2</v>
+      </c>
+      <c r="BZ14" s="8">
+        <f t="shared" ref="BZ14:BZ16" si="100">AR14+BI14</f>
+        <v>9.9999992018484196E-2</v>
+      </c>
+      <c r="CA14" s="8">
+        <f t="shared" si="62"/>
+        <v>9.9999992018484196E-2</v>
+      </c>
+      <c r="CB14" s="8">
+        <f t="shared" si="63"/>
+        <v>9.9999990997061208E-2</v>
+      </c>
+      <c r="CC14" s="8">
+        <f t="shared" si="64"/>
+        <v>9.9999990997061208E-2</v>
+      </c>
+      <c r="CD14" s="8">
+        <f t="shared" si="65"/>
+        <v>9.9999999902185263E-2</v>
+      </c>
+      <c r="CE14" s="8">
+        <f t="shared" si="66"/>
+        <v>9.9999999902185263E-2</v>
+      </c>
+      <c r="CF14" s="8">
+        <f t="shared" si="67"/>
+        <v>6.2898733887847239E-2</v>
+      </c>
+      <c r="CG14" s="8">
+        <f t="shared" si="68"/>
+        <v>0.11494193775853398</v>
+      </c>
+      <c r="CH14" s="8">
+        <f t="shared" si="69"/>
+        <v>6.2898733887847239E-2</v>
+      </c>
+      <c r="CI14" s="8">
+        <f t="shared" si="70"/>
+        <v>0.11494193775853398</v>
+      </c>
+      <c r="CJ14" s="5">
+        <f t="shared" si="71"/>
+        <v>0.1</v>
+      </c>
+      <c r="CK14" s="5">
+        <f t="shared" si="72"/>
+        <v>0.1</v>
+      </c>
+      <c r="CL14" s="5">
+        <f t="shared" si="73"/>
+        <v>0.11508915090845562</v>
+      </c>
+      <c r="CM14" s="8">
+        <f t="shared" si="74"/>
+        <v>9.9999999899070671E-2</v>
+      </c>
+      <c r="CN14" s="8">
+        <f t="shared" si="75"/>
+        <v>9.9999999899070671E-2</v>
+      </c>
+      <c r="CO14" s="8">
+        <f t="shared" si="76"/>
+        <v>6.2898732750485811E-2</v>
+      </c>
+      <c r="CP14" s="8">
+        <f t="shared" si="77"/>
+        <v>0.11494193805035249</v>
+      </c>
+    </row>
+    <row r="15" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K15" s="20"/>
+      <c r="L15" s="11">
+        <v>83</v>
+      </c>
+      <c r="M15" s="11">
+        <v>86</v>
+      </c>
+      <c r="N15" s="11">
+        <v>1</v>
+      </c>
+      <c r="O15" s="11">
+        <v>0</v>
+      </c>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="8">
+        <f t="shared" si="78"/>
+        <v>17.099998563082707</v>
+      </c>
+      <c r="T15" s="8">
+        <f t="shared" si="79"/>
+        <v>17.099998563082707</v>
+      </c>
+      <c r="U15" s="8">
+        <f t="shared" si="80"/>
+        <v>0.18869619581383762</v>
+      </c>
+      <c r="V15" s="8">
+        <f t="shared" si="81"/>
+        <v>0.34482580495602611</v>
+      </c>
+      <c r="W15" s="11">
+        <f t="shared" si="82"/>
+        <v>83</v>
+      </c>
+      <c r="X15" s="11">
+        <f t="shared" si="83"/>
+        <v>86</v>
+      </c>
+      <c r="Y15" s="11">
+        <f t="shared" si="84"/>
+        <v>1</v>
+      </c>
+      <c r="Z15" s="8">
+        <f t="shared" si="85"/>
+        <v>0.99999996254024215</v>
+      </c>
+      <c r="AA15" s="8">
+        <f t="shared" si="86"/>
+        <v>0.99999996254024215</v>
+      </c>
+      <c r="AB15" s="8">
+        <f t="shared" si="87"/>
+        <v>0.54703457129477451</v>
+      </c>
+      <c r="AC15" s="8">
+        <f t="shared" si="88"/>
+        <v>0.58536229030786791</v>
+      </c>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="15"/>
+      <c r="AF15" s="15"/>
+      <c r="AG15" s="15"/>
+      <c r="AH15" s="15"/>
+      <c r="AI15" s="8">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="8">
+        <f t="shared" si="89"/>
+        <v>4.7271449277822639E-7</v>
+      </c>
+      <c r="AL15" s="8">
+        <f t="shared" si="90"/>
+        <v>5.0772008623466385E-7</v>
+      </c>
+      <c r="AM15" s="8">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="AN15" s="8">
+        <f t="shared" si="92"/>
+        <v>-3.4727779202763102E-10</v>
+      </c>
+      <c r="AO15" s="8">
+        <f t="shared" si="93"/>
+        <v>-3.4727779202763102E-10</v>
+      </c>
+      <c r="AP15" s="8">
+        <f t="shared" si="94"/>
+        <v>0.11223928400039614</v>
+      </c>
+      <c r="AQ15" s="8">
+        <f t="shared" si="95"/>
+        <v>-0.1420752011138513</v>
+      </c>
+      <c r="AR15" s="8">
+        <f t="shared" si="96"/>
+        <v>9.9999992018484196E-2</v>
+      </c>
+      <c r="AS15" s="8">
+        <f t="shared" si="22"/>
+        <v>9.9999992018484196E-2</v>
+      </c>
+      <c r="AT15" s="8">
+        <f t="shared" si="23"/>
+        <v>9.9999990997061208E-2</v>
+      </c>
+      <c r="AU15" s="8">
+        <f t="shared" si="24"/>
+        <v>9.9999990997061208E-2</v>
+      </c>
+      <c r="AV15" s="8">
+        <f t="shared" si="25"/>
+        <v>9.9999999902185263E-2</v>
+      </c>
+      <c r="AW15" s="8">
+        <f t="shared" si="26"/>
+        <v>9.9999999902185263E-2</v>
+      </c>
+      <c r="AX15" s="8">
+        <f t="shared" si="27"/>
+        <v>6.2898733887847239E-2</v>
+      </c>
+      <c r="AY15" s="8">
+        <f t="shared" si="28"/>
+        <v>0.11494193775853398</v>
+      </c>
+      <c r="AZ15" s="8">
+        <f t="shared" si="29"/>
+        <v>6.2898733887847239E-2</v>
+      </c>
+      <c r="BA15" s="8">
+        <f t="shared" si="30"/>
+        <v>0.11494193775853398</v>
+      </c>
+      <c r="BB15" s="5">
+        <f t="shared" si="31"/>
+        <v>0.1</v>
+      </c>
+      <c r="BC15" s="5">
+        <f t="shared" si="32"/>
+        <v>0.1</v>
+      </c>
+      <c r="BD15" s="5">
+        <f t="shared" si="33"/>
+        <v>0.11508915090845562</v>
+      </c>
+      <c r="BE15" s="8">
+        <f t="shared" si="34"/>
+        <v>9.9999999899070671E-2</v>
+      </c>
+      <c r="BF15" s="8">
+        <f t="shared" si="35"/>
+        <v>9.9999999899070671E-2</v>
+      </c>
+      <c r="BG15" s="8">
+        <f t="shared" si="36"/>
+        <v>6.2898732750485811E-2</v>
+      </c>
+      <c r="BH15" s="8">
+        <f t="shared" si="37"/>
+        <v>0.11494193805035249</v>
+      </c>
+      <c r="BI15" s="8">
+        <f t="shared" ref="BI15:BI16" si="101">$L$2*AN15*W15+$L$3*BI14</f>
+        <v>-2.8927741083771527E-9</v>
+      </c>
+      <c r="BJ15" s="8">
+        <f t="shared" ref="BJ15:BJ16" si="102">$L$2*AO15*W15+$L$3*BJ14</f>
+        <v>-2.8927741083771527E-9</v>
+      </c>
+      <c r="BK15" s="8">
+        <f t="shared" ref="BK15:BK16" si="103">$L$2*AN15*X15+BK14*$L$3</f>
+        <v>-2.9971692657614535E-9</v>
+      </c>
+      <c r="BL15" s="8">
+        <f t="shared" ref="BL15:BL16" si="104">$L$2*AO15*X15+BL14*$L$3</f>
+        <v>-2.9971692657614535E-9</v>
+      </c>
+      <c r="BM15" s="8">
+        <f t="shared" ref="BM15:BM16" si="105">$L$2*AN15*Y15+BM14*$L$3</f>
+        <v>-3.4829824806759843E-11</v>
+      </c>
+      <c r="BN15" s="8">
+        <f t="shared" ref="BN15:BN16" si="106">$L$2*AO15*Y15+BN14*$L$3</f>
+        <v>-3.4829824806759843E-11</v>
+      </c>
+      <c r="BO15" s="8">
+        <f t="shared" ref="BO15:BO16" si="107">$L$2*AP15*Z15+BO14*$L$3</f>
+        <v>9.7077219251537374E-3</v>
+      </c>
+      <c r="BP15" s="8">
+        <f t="shared" ref="BP15:BP16" si="108">$L$2*AQ15*Z15+BP14*$L$3</f>
+        <v>-1.306965964240123E-2</v>
+      </c>
+      <c r="BQ15" s="8">
+        <f t="shared" ref="BQ15:BQ16" si="109">$L$2*AP15*AA15+BQ14*$L$3</f>
+        <v>9.7077219251537374E-3</v>
+      </c>
+      <c r="BR15" s="8">
+        <f t="shared" ref="BR15:BR16" si="110">$L$2*AQ15*AA15+BR14*$L$3</f>
+        <v>-1.306965964240123E-2</v>
+      </c>
+      <c r="BS15" s="5">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="BT15" s="5">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="BU15" s="5">
+        <f t="shared" si="99"/>
+        <v>6.2898733887847245E-3</v>
+      </c>
+      <c r="BV15" s="8">
+        <f t="shared" ref="BV15:BV16" si="111">$L$2*AN15*$L$4+BV14*$L$3</f>
+        <v>-3.4851006784360994E-11</v>
+      </c>
+      <c r="BW15" s="8">
+        <f t="shared" ref="BW15:BW16" si="112">$L$2*AO15*$L$4+BW14*$L$3</f>
+        <v>-3.4851006784360994E-11</v>
+      </c>
+      <c r="BX15" s="8">
+        <f t="shared" ref="BX15:BX16" si="113">$L$2*AP15*$L$4+BX14*$L$3</f>
+        <v>9.7077222892998395E-3</v>
+      </c>
+      <c r="BY15" s="8">
+        <f t="shared" ref="BY15:BY16" si="114">$L$2*AQ15*$L$4+BY14*$L$3</f>
+        <v>-1.3069660132363995E-2</v>
+      </c>
+      <c r="BZ15" s="8">
+        <f t="shared" si="100"/>
+        <v>9.9999989125710093E-2</v>
+      </c>
+      <c r="CA15" s="8">
+        <f t="shared" si="62"/>
+        <v>9.9999989125710093E-2</v>
+      </c>
+      <c r="CB15" s="8">
+        <f t="shared" si="63"/>
+        <v>9.9999987999891946E-2</v>
+      </c>
+      <c r="CC15" s="8">
+        <f t="shared" si="64"/>
+        <v>9.9999987999891946E-2</v>
+      </c>
+      <c r="CD15" s="8">
+        <f t="shared" si="65"/>
+        <v>9.9999999867355444E-2</v>
+      </c>
+      <c r="CE15" s="8">
+        <f t="shared" si="66"/>
+        <v>9.9999999867355444E-2</v>
+      </c>
+      <c r="CF15" s="8">
+        <f t="shared" si="67"/>
+        <v>7.2606455813000972E-2</v>
+      </c>
+      <c r="CG15" s="8">
+        <f t="shared" si="68"/>
+        <v>0.10187227811613275</v>
+      </c>
+      <c r="CH15" s="8">
+        <f t="shared" si="69"/>
+        <v>7.2606455813000972E-2</v>
+      </c>
+      <c r="CI15" s="8">
+        <f t="shared" si="70"/>
+        <v>0.10187227811613275</v>
+      </c>
+      <c r="CJ15" s="5">
+        <f t="shared" si="71"/>
+        <v>0.1</v>
+      </c>
+      <c r="CK15" s="5">
+        <f t="shared" si="72"/>
+        <v>0.1</v>
+      </c>
+      <c r="CL15" s="5">
+        <f t="shared" si="73"/>
+        <v>0.12137902429724035</v>
+      </c>
+      <c r="CM15" s="8">
+        <f t="shared" si="74"/>
+        <v>9.999999986421966E-2</v>
+      </c>
+      <c r="CN15" s="8">
+        <f t="shared" si="75"/>
+        <v>9.999999986421966E-2</v>
+      </c>
+      <c r="CO15" s="8">
+        <f t="shared" si="76"/>
+        <v>7.2606455039785647E-2</v>
+      </c>
+      <c r="CP15" s="8">
+        <f t="shared" si="77"/>
+        <v>0.1018722779179885</v>
+      </c>
+    </row>
+    <row r="16" spans="11:94" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="20"/>
+      <c r="L16" s="6">
+        <v>70</v>
+      </c>
+      <c r="M16" s="6">
+        <v>96</v>
+      </c>
+      <c r="N16" s="6">
+        <v>1</v>
+      </c>
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="9">
+        <f t="shared" si="78"/>
+        <v>16.799998086520908</v>
+      </c>
+      <c r="T16" s="9">
+        <f t="shared" si="79"/>
+        <v>16.799998086520908</v>
+      </c>
+      <c r="U16" s="9">
+        <f t="shared" si="80"/>
+        <v>0.21781935932303753</v>
+      </c>
+      <c r="V16" s="9">
+        <f t="shared" si="81"/>
+        <v>0.30561682384782746</v>
+      </c>
+      <c r="W16" s="12">
+        <f t="shared" si="82"/>
+        <v>70</v>
+      </c>
+      <c r="X16" s="12">
+        <f t="shared" si="83"/>
+        <v>96</v>
+      </c>
+      <c r="Y16" s="12">
+        <f t="shared" si="84"/>
+        <v>1</v>
+      </c>
+      <c r="Z16" s="9">
+        <f t="shared" si="85"/>
+        <v>0.99999994943459225</v>
+      </c>
+      <c r="AA16" s="9">
+        <f t="shared" si="86"/>
+        <v>0.99999994943459225</v>
+      </c>
+      <c r="AB16" s="9">
+        <f t="shared" si="87"/>
+        <v>0.55424055439330799</v>
+      </c>
+      <c r="AC16" s="9">
+        <f t="shared" si="88"/>
+        <v>0.5758150185933153</v>
+      </c>
+      <c r="AD16" s="16"/>
+      <c r="AE16" s="16"/>
+      <c r="AF16" s="16"/>
+      <c r="AG16" s="16"/>
+      <c r="AH16" s="16"/>
+      <c r="AI16" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="9">
+        <f t="shared" si="89"/>
+        <v>3.0927895243020585E-7</v>
+      </c>
+      <c r="AL16" s="9">
+        <f t="shared" si="90"/>
+        <v>5.8398012720670309E-7</v>
+      </c>
+      <c r="AM16" s="9">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="AN16" s="9">
+        <f t="shared" si="92"/>
+        <v>-3.2016458184482338E-10</v>
+      </c>
+      <c r="AO16" s="9">
+        <f t="shared" si="93"/>
+        <v>-3.2016458184482338E-10</v>
+      </c>
+      <c r="AP16" s="9">
+        <f t="shared" si="94"/>
+        <v>0.11012842028933839</v>
+      </c>
+      <c r="AQ16" s="9">
+        <f t="shared" si="95"/>
+        <v>-0.14064401768858964</v>
+      </c>
+      <c r="AR16" s="9">
+        <f t="shared" si="96"/>
+        <v>9.9999989125710093E-2</v>
+      </c>
+      <c r="AS16" s="9">
+        <f t="shared" si="22"/>
+        <v>9.9999989125710093E-2</v>
+      </c>
+      <c r="AT16" s="9">
+        <f t="shared" si="23"/>
+        <v>9.9999987999891946E-2</v>
+      </c>
+      <c r="AU16" s="9">
+        <f t="shared" si="24"/>
+        <v>9.9999987999891946E-2</v>
+      </c>
+      <c r="AV16" s="9">
+        <f t="shared" si="25"/>
+        <v>9.9999999867355444E-2</v>
+      </c>
+      <c r="AW16" s="9">
+        <f t="shared" si="26"/>
+        <v>9.9999999867355444E-2</v>
+      </c>
+      <c r="AX16" s="9">
+        <f t="shared" si="27"/>
+        <v>7.2606455813000972E-2</v>
+      </c>
+      <c r="AY16" s="9">
+        <f t="shared" si="28"/>
+        <v>0.10187227811613275</v>
+      </c>
+      <c r="AZ16" s="9">
+        <f t="shared" si="29"/>
+        <v>7.2606455813000972E-2</v>
+      </c>
+      <c r="BA16" s="9">
+        <f t="shared" si="30"/>
+        <v>0.10187227811613275</v>
+      </c>
+      <c r="BB16" s="7">
+        <f t="shared" si="31"/>
+        <v>0.1</v>
+      </c>
+      <c r="BC16" s="7">
+        <f t="shared" si="32"/>
+        <v>0.1</v>
+      </c>
+      <c r="BD16" s="7">
+        <f t="shared" si="33"/>
+        <v>0.12137902429724035</v>
+      </c>
+      <c r="BE16" s="9">
+        <f t="shared" si="34"/>
+        <v>9.999999986421966E-2</v>
+      </c>
+      <c r="BF16" s="9">
+        <f t="shared" si="35"/>
+        <v>9.999999986421966E-2</v>
+      </c>
+      <c r="BG16" s="9">
+        <f t="shared" si="36"/>
+        <v>7.2606455039785647E-2</v>
+      </c>
+      <c r="BH16" s="9">
+        <f t="shared" si="37"/>
+        <v>0.1018722779179885</v>
+      </c>
+      <c r="BI16" s="9">
+        <f t="shared" si="101"/>
+        <v>-2.5304294837514792E-9</v>
+      </c>
+      <c r="BJ16" s="9">
+        <f t="shared" si="102"/>
+        <v>-2.5304294837514792E-9</v>
+      </c>
+      <c r="BK16" s="9">
+        <f t="shared" si="103"/>
+        <v>-3.3732969122864496E-9</v>
+      </c>
+      <c r="BL16" s="9">
+        <f t="shared" si="104"/>
+        <v>-3.3732969122864496E-9</v>
+      </c>
+      <c r="BM16" s="9">
+        <f t="shared" si="105"/>
+        <v>-3.5499440665158323E-11</v>
+      </c>
+      <c r="BN16" s="9">
+        <f t="shared" si="106"/>
+        <v>-3.5499440665158323E-11</v>
+      </c>
+      <c r="BO16" s="9">
+        <f t="shared" si="107"/>
+        <v>1.1983613664580365E-2</v>
+      </c>
+      <c r="BP16" s="9">
+        <f t="shared" si="108"/>
+        <v>-1.5371367021926879E-2</v>
+      </c>
+      <c r="BQ16" s="9">
+        <f t="shared" si="109"/>
+        <v>1.1983613664580365E-2</v>
+      </c>
+      <c r="BR16" s="9">
+        <f t="shared" si="110"/>
+        <v>-1.5371367021926879E-2</v>
+      </c>
+      <c r="BS16" s="7">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="BT16" s="7">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="BU16" s="7">
+        <f t="shared" si="99"/>
+        <v>7.2606455813000979E-3</v>
+      </c>
+      <c r="BV16" s="9">
+        <f t="shared" si="111"/>
+        <v>-3.5501558862918435E-11</v>
+      </c>
+      <c r="BW16" s="9">
+        <f t="shared" si="112"/>
+        <v>-3.5501558862918435E-11</v>
+      </c>
+      <c r="BX16" s="9">
+        <f t="shared" si="113"/>
+        <v>1.1983614257863824E-2</v>
+      </c>
+      <c r="BY16" s="9">
+        <f t="shared" si="114"/>
+        <v>-1.5371367782095365E-2</v>
+      </c>
+      <c r="BZ16" s="9">
+        <f t="shared" si="100"/>
+        <v>9.9999986595280616E-2</v>
+      </c>
+      <c r="CA16" s="9">
+        <f t="shared" si="62"/>
+        <v>9.9999986595280616E-2</v>
+      </c>
+      <c r="CB16" s="9">
+        <f t="shared" si="63"/>
+        <v>9.999998462659504E-2</v>
+      </c>
+      <c r="CC16" s="9">
+        <f t="shared" si="64"/>
+        <v>9.999998462659504E-2</v>
+      </c>
+      <c r="CD16" s="9">
+        <f t="shared" si="65"/>
+        <v>9.9999999831856007E-2</v>
+      </c>
+      <c r="CE16" s="9">
+        <f t="shared" si="66"/>
+        <v>9.9999999831856007E-2</v>
+      </c>
+      <c r="CF16" s="9">
+        <f t="shared" si="67"/>
+        <v>8.4590069477581339E-2</v>
+      </c>
+      <c r="CG16" s="9">
+        <f t="shared" si="68"/>
+        <v>8.6500911094205879E-2</v>
+      </c>
+      <c r="CH16" s="9">
+        <f t="shared" si="69"/>
+        <v>8.4590069477581339E-2</v>
+      </c>
+      <c r="CI16" s="9">
+        <f t="shared" si="70"/>
+        <v>8.6500911094205879E-2</v>
+      </c>
+      <c r="CJ16" s="7">
+        <f t="shared" si="71"/>
+        <v>0.1</v>
+      </c>
+      <c r="CK16" s="7">
+        <f t="shared" si="72"/>
+        <v>0.1</v>
+      </c>
+      <c r="CL16" s="7">
+        <f t="shared" si="73"/>
+        <v>0.12863966987854045</v>
+      </c>
+      <c r="CM16" s="9">
+        <f t="shared" si="74"/>
+        <v>9.99999998287181E-2</v>
+      </c>
+      <c r="CN16" s="9">
+        <f t="shared" si="75"/>
+        <v>9.99999998287181E-2</v>
+      </c>
+      <c r="CO16" s="9">
+        <f t="shared" si="76"/>
+        <v>8.4590069297649478E-2</v>
+      </c>
+      <c r="CP16" s="9">
+        <f t="shared" si="77"/>
+        <v>8.6500910135893144E-2</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="K9:K12"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="M6:M8"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="O6:O8"/>
-    <mergeCell ref="K6:K8"/>
+  <mergeCells count="16">
+    <mergeCell ref="K13:K16"/>
     <mergeCell ref="BZ7:CP7"/>
     <mergeCell ref="AR6:CP6"/>
     <mergeCell ref="P6:AQ6"/>
@@ -2415,6 +3623,12 @@
     <mergeCell ref="AD7:AJ7"/>
     <mergeCell ref="AR7:BH7"/>
     <mergeCell ref="BI7:BY7"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="K6:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>